<commit_message>
finished manual data measurement and data entry for first 95 parks
</commit_message>
<xml_diff>
--- a/data/google_earth_manual.xlsx
+++ b/data/google_earth_manual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\Baseball_fields\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\BB_parks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D787B4-5109-449D-8DAD-85326C5F4557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8855999-F132-422A-A29D-7B300E30E153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{810870C9-568A-4025-AECC-CEADD1B80506}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="119">
   <si>
     <t>Detroit Western</t>
   </si>
@@ -173,6 +173,225 @@
   </si>
   <si>
     <t>Foul_pct_of_whole</t>
+  </si>
+  <si>
+    <t>Homer High School</t>
+  </si>
+  <si>
+    <t>Blissfield High School</t>
+  </si>
+  <si>
+    <t>Westside Park - Lansing</t>
+  </si>
+  <si>
+    <t>Turtle Creek Stadium - Traverse City</t>
+  </si>
+  <si>
+    <t>1. Grosse Pointe Woods University Liggett</t>
+  </si>
+  <si>
+    <t>1. Buchanan</t>
+  </si>
+  <si>
+    <t>3. Hemlock</t>
+  </si>
+  <si>
+    <t>4. Chesaning</t>
+  </si>
+  <si>
+    <t>5. Standish-Sterling</t>
+  </si>
+  <si>
+    <t>6. New Lothrop</t>
+  </si>
+  <si>
+    <t>7. Bridgman</t>
+  </si>
+  <si>
+    <t>8. Watervliet</t>
+  </si>
+  <si>
+    <t>9. Bad Axe</t>
+  </si>
+  <si>
+    <t>10. Jackson Lumen Christi</t>
+  </si>
+  <si>
+    <t>1. Beal City</t>
+  </si>
+  <si>
+    <t>2. Royal Oak Shrine</t>
+  </si>
+  <si>
+    <t>3. Rudyard</t>
+  </si>
+  <si>
+    <t>4. Maple City Glen Lake</t>
+  </si>
+  <si>
+    <t>5. Rogers City</t>
+  </si>
+  <si>
+    <t>6. Rochester Hills Lutheran Northwest</t>
+  </si>
+  <si>
+    <t>7. Indian River Inland Lakes</t>
+  </si>
+  <si>
+    <t>8. Breckenridge</t>
+  </si>
+  <si>
+    <t>9. Marine City Cardinal Mooney</t>
+  </si>
+  <si>
+    <t>10. Kalamazoo Christian</t>
+  </si>
+  <si>
+    <t>Marine City Cardinal Mooney - PRACTICE</t>
+  </si>
+  <si>
+    <t>Jimmy John's Stadium - Utica</t>
+  </si>
+  <si>
+    <t>U of M</t>
+  </si>
+  <si>
+    <t>EMU</t>
+  </si>
+  <si>
+    <t>CMU</t>
+  </si>
+  <si>
+    <t>WMU</t>
+  </si>
+  <si>
+    <t>GVSU</t>
+  </si>
+  <si>
+    <t>Dow Diamond - Midland</t>
+  </si>
+  <si>
+    <t>West Michigan Whitecaps</t>
+  </si>
+  <si>
+    <t>Sag Vally State</t>
+  </si>
+  <si>
+    <t>Davenport University</t>
+  </si>
+  <si>
+    <t>pro</t>
+  </si>
+  <si>
+    <t>college</t>
+  </si>
+  <si>
+    <t>Moose Lodge - Lansing</t>
+  </si>
+  <si>
+    <t>St. Gerrard 1 - Lansing</t>
+  </si>
+  <si>
+    <t>Battle Creek - Bailey</t>
+  </si>
+  <si>
+    <t>Kalamazoo Growlers</t>
+  </si>
+  <si>
+    <t>Hamtramck Historical</t>
+  </si>
+  <si>
+    <t>Marsh Field - Muskegon</t>
+  </si>
+  <si>
+    <t>Grand Ledge MS - 14u</t>
+  </si>
+  <si>
+    <t>Grand Ledge Hayes - 12u</t>
+  </si>
+  <si>
+    <t>Grand Ledge Bridge Park - 10u</t>
+  </si>
+  <si>
+    <t>St. Gerrard 2 - Lansing</t>
+  </si>
+  <si>
+    <t>Hamtramck Park 2 - school</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t>semi-pro</t>
+  </si>
+  <si>
+    <t>muni</t>
+  </si>
+  <si>
+    <t>high school</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>1. Ada Forest Hills Eastern</t>
+  </si>
+  <si>
+    <t>2. New Boston Huron</t>
+  </si>
+  <si>
+    <t>3. Detroit Country Day</t>
+  </si>
+  <si>
+    <t>4. Goodrich</t>
+  </si>
+  <si>
+    <t>5. Midland Bullock Creek</t>
+  </si>
+  <si>
+    <t>6. Richmond</t>
+  </si>
+  <si>
+    <t>7. St. Clair</t>
+  </si>
+  <si>
+    <t>8. Essexville Garber</t>
+  </si>
+  <si>
+    <t>9. Cheboygan</t>
+  </si>
+  <si>
+    <t>10. Eaton Rapids</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>14u</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>12u</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Owosso HS</t>
+  </si>
+  <si>
+    <t>Pewamo Westphalia</t>
   </si>
 </sst>
 </file>
@@ -181,7 +400,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -224,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,24 +759,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995A9B2-ED22-410A-BC8E-AC27A4E2E923}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -582,8 +803,14 @@
       <c r="I1" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -614,8 +841,14 @@
         <f>E2/(E2+C2)</f>
         <v>0.29936761020569486</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -635,19 +868,25 @@
         <v>1332</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G39" si="0">C3/D3</f>
+        <f t="shared" ref="G3:G55" si="0">C3/D3</f>
         <v>73.918777292576422</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H39" si="1">E3/F3</f>
+        <f t="shared" ref="H3:H55" si="1">E3/F3</f>
         <v>15.311561561561561</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I39" si="2">E3/(E3+C3)</f>
+        <f t="shared" ref="I3:I55" si="2">E3/(E3+C3)</f>
         <v>0.19417891690151573</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -678,8 +917,14 @@
         <f t="shared" si="2"/>
         <v>0.30607622492916942</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -710,8 +955,17 @@
         <f t="shared" si="2"/>
         <v>0.268331274248434</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -742,8 +996,14 @@
         <f t="shared" si="2"/>
         <v>0.28540637553779447</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -774,8 +1034,14 @@
         <f t="shared" si="2"/>
         <v>0.28295894119185128</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -806,8 +1072,14 @@
         <f t="shared" si="2"/>
         <v>0.28650556896370805</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -838,8 +1110,14 @@
         <f t="shared" si="2"/>
         <v>0.28840544924247385</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -870,8 +1148,14 @@
         <f t="shared" si="2"/>
         <v>0.17278518421225456</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -902,8 +1186,14 @@
         <f t="shared" si="2"/>
         <v>0.27840379118399278</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -934,8 +1224,14 @@
         <f t="shared" si="2"/>
         <v>0.25905807715163331</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -966,8 +1262,14 @@
         <f t="shared" si="2"/>
         <v>0.2590617373226069</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -998,8 +1300,14 @@
         <f t="shared" si="2"/>
         <v>0.20818931576111732</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1030,8 +1338,14 @@
         <f t="shared" si="2"/>
         <v>0.25798121863675877</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1062,8 +1376,14 @@
         <f t="shared" si="2"/>
         <v>0.23842243735472171</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1094,8 +1414,14 @@
         <f t="shared" si="2"/>
         <v>0.14410110711621787</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1126,8 +1452,14 @@
         <f t="shared" si="2"/>
         <v>0.2047791144776144</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1158,8 +1490,14 @@
         <f t="shared" si="2"/>
         <v>0.26651598799510912</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1190,8 +1528,11 @@
         <f t="shared" si="2"/>
         <v>0.21870804502736754</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1222,8 +1563,14 @@
         <f t="shared" si="2"/>
         <v>0.23882081304750127</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1254,8 +1601,14 @@
         <f t="shared" si="2"/>
         <v>0.23952195866177486</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1286,8 +1639,14 @@
         <f t="shared" si="2"/>
         <v>0.17875952465553319</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>81</v>
+      </c>
+      <c r="K23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1318,8 +1677,14 @@
         <f t="shared" si="2"/>
         <v>0.3094735690393573</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1350,8 +1715,14 @@
         <f t="shared" si="2"/>
         <v>0.25748487882025356</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>97</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1382,8 +1753,11 @@
         <f t="shared" si="2"/>
         <v>0.17295685478934575</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1414,8 +1788,14 @@
         <f t="shared" si="2"/>
         <v>0.20872751702446027</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>97</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1446,8 +1826,14 @@
         <f t="shared" si="2"/>
         <v>0.19855810008481764</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1478,8 +1864,14 @@
         <f t="shared" si="2"/>
         <v>0.2642204977061533</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>97</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1510,8 +1902,17 @@
         <f t="shared" si="2"/>
         <v>0.23743744787322768</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>97</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1542,8 +1943,17 @@
         <f t="shared" si="2"/>
         <v>0.23080261349663669</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>97</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1574,8 +1984,17 @@
         <f t="shared" si="2"/>
         <v>0.26542539394332404</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>97</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1606,8 +2025,17 @@
         <f t="shared" si="2"/>
         <v>0.22153853881507898</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>97</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1638,8 +2066,17 @@
         <f t="shared" si="2"/>
         <v>0.28808258459185626</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>97</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1670,8 +2107,17 @@
         <f t="shared" si="2"/>
         <v>0.23944766088795616</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>97</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1702,8 +2148,17 @@
         <f t="shared" si="2"/>
         <v>0.26757583647962507</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>97</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1734,8 +2189,17 @@
         <f t="shared" si="2"/>
         <v>0.29298206333806004</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>97</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1766,8 +2230,17 @@
         <f t="shared" si="2"/>
         <v>0.185067074295654</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>97</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1798,8 +2271,2063 @@
         <f t="shared" si="2"/>
         <v>0.21042414475130028</v>
       </c>
+      <c r="J39" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="2">
+        <v>71699</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1062</v>
+      </c>
+      <c r="E40" s="2">
+        <v>20789</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1297</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="0"/>
+        <v>67.513182674199626</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="1"/>
+        <v>16.028527370855819</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22477510595969208</v>
+      </c>
+      <c r="J40" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="2">
+        <v>92143</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1190</v>
+      </c>
+      <c r="E41" s="2">
+        <v>20350</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1371</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="0"/>
+        <v>77.431092436974794</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>14.843180160466813</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="2"/>
+        <v>0.18090014489790476</v>
+      </c>
+      <c r="J41" t="s">
+        <v>97</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="2">
+        <v>96413</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1220</v>
+      </c>
+      <c r="E42" s="2">
+        <v>37308</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1525</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="0"/>
+        <v>79.027049180327865</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>24.464262295081966</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="2"/>
+        <v>0.27899881095714213</v>
+      </c>
+      <c r="J42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="2">
+        <v>109576</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1258</v>
+      </c>
+      <c r="E43" s="2">
+        <v>29577</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1401</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
+        <v>87.103338632750393</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>21.111349036402569</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.21255021451208383</v>
+      </c>
+      <c r="J43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="2">
+        <v>82933</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1145</v>
+      </c>
+      <c r="E44" s="2">
+        <v>22338</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1309</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="0"/>
+        <v>72.430567685589523</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>17.064935064935064</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="2"/>
+        <v>0.21219519145823637</v>
+      </c>
+      <c r="J44" t="s">
+        <v>97</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="2">
+        <v>88278</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1197</v>
+      </c>
+      <c r="E45" s="2">
+        <v>22609</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1623</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="0"/>
+        <v>73.749373433583955</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>13.930375847196549</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="2"/>
+        <v>0.20389225066960059</v>
+      </c>
+      <c r="J45" t="s">
+        <v>97</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <v>86966</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1149</v>
+      </c>
+      <c r="E46" s="2">
+        <v>24774</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1354</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="0"/>
+        <v>75.688424717145338</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="1"/>
+        <v>18.296898079763665</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22171111508859853</v>
+      </c>
+      <c r="J46" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="L46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="2">
+        <v>93229</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1200</v>
+      </c>
+      <c r="E47" s="2">
+        <v>42614</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1524</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="0"/>
+        <v>77.69083333333333</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="1"/>
+        <v>27.961942257217849</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="2"/>
+        <v>0.31370037469726081</v>
+      </c>
+      <c r="J47" t="s">
+        <v>97</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="L47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="2">
+        <v>95281</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1187</v>
+      </c>
+      <c r="E48" s="2">
+        <v>27551</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1377</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="0"/>
+        <v>80.27042965459141</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>20.007988380537402</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22429822847466457</v>
+      </c>
+      <c r="J48" t="s">
+        <v>97</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="2">
+        <v>89268</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1168</v>
+      </c>
+      <c r="E49" s="2">
+        <v>37330</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1417</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="0"/>
+        <v>76.428082191780817</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>26.344389555398731</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="2"/>
+        <v>0.2948703770991643</v>
+      </c>
+      <c r="J49" t="s">
+        <v>97</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="2">
+        <v>93886</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1206</v>
+      </c>
+      <c r="E50" s="2">
+        <v>29234</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1416</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="0"/>
+        <v>77.849087893864009</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="1"/>
+        <v>20.645480225988699</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="2"/>
+        <v>0.23744314489928525</v>
+      </c>
+      <c r="J50" t="s">
+        <v>97</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="2">
+        <v>90554</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1175</v>
+      </c>
+      <c r="E51" s="2">
+        <v>29910</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1400</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="0"/>
+        <v>77.067234042553196</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>21.364285714285714</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="2"/>
+        <v>0.24828994554389694</v>
+      </c>
+      <c r="J51" t="s">
+        <v>97</v>
+      </c>
+      <c r="K51">
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="2">
+        <v>86081</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1150</v>
+      </c>
+      <c r="E52" s="2">
+        <v>38759</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1441</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="0"/>
+        <v>74.853043478260872</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="1"/>
+        <v>26.897293546148507</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="2"/>
+        <v>0.31046940083306634</v>
+      </c>
+      <c r="J52" t="s">
+        <v>97</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="2">
+        <v>91826</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1167</v>
+      </c>
+      <c r="E53" s="2">
+        <v>20452</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1318</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="0"/>
+        <v>78.685518423307627</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="1"/>
+        <v>15.517450682852807</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="2"/>
+        <v>0.18215500810488253</v>
+      </c>
+      <c r="J53" t="s">
+        <v>97</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="2">
+        <v>89288</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1177</v>
+      </c>
+      <c r="E54" s="2">
+        <v>25641</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1414</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="0"/>
+        <v>75.860662701784193</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="1"/>
+        <v>18.133663366336634</v>
+      </c>
+      <c r="I54" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22310295921830001</v>
+      </c>
+      <c r="J54" t="s">
+        <v>97</v>
+      </c>
+      <c r="K54">
+        <v>4</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="2">
+        <v>97285</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1243</v>
+      </c>
+      <c r="E55" s="2">
+        <v>14680</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1381</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="0"/>
+        <v>78.266291230893003</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="1"/>
+        <v>10.629978276611151</v>
+      </c>
+      <c r="I55" s="3">
+        <f t="shared" si="2"/>
+        <v>0.13111240119680256</v>
+      </c>
+      <c r="J55" t="s">
+        <v>97</v>
+      </c>
+      <c r="K55">
+        <v>4</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="2">
+        <v>85108</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1143</v>
+      </c>
+      <c r="E56" s="2">
+        <v>26111</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1346</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" ref="G56:G94" si="3">C56/D56</f>
+        <v>74.460192475940502</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" ref="H56:H94" si="4">E56/F56</f>
+        <v>19.398959881129272</v>
+      </c>
+      <c r="I56" s="3">
+        <f t="shared" ref="I56:I94" si="5">E56/(E56+C56)</f>
+        <v>0.23477103732275961</v>
+      </c>
+      <c r="J56" t="s">
+        <v>97</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+      <c r="L56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="2">
+        <v>92201</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1228</v>
+      </c>
+      <c r="E57" s="2">
+        <v>23386</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1466</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="3"/>
+        <v>75.082247557003257</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="4"/>
+        <v>15.95225102319236</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" si="5"/>
+        <v>0.20232379073771273</v>
+      </c>
+      <c r="J57" t="s">
+        <v>97</v>
+      </c>
+      <c r="K57">
+        <v>4</v>
+      </c>
+      <c r="L57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="2">
+        <v>71715</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1079</v>
+      </c>
+      <c r="E58" s="2">
+        <v>18494</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1306</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="3"/>
+        <v>66.464318813716403</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="4"/>
+        <v>14.160796324655436</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="5"/>
+        <v>0.20501280360052768</v>
+      </c>
+      <c r="J58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K58">
+        <v>4</v>
+      </c>
+      <c r="L58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="2">
+        <v>70894</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1046</v>
+      </c>
+      <c r="E59" s="2">
+        <v>19743</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1270</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="3"/>
+        <v>67.77629063097514</v>
+      </c>
+      <c r="H59" s="1">
+        <f t="shared" si="4"/>
+        <v>15.545669291338582</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="5"/>
+        <v>0.2178249500755762</v>
+      </c>
+      <c r="J59" t="s">
+        <v>97</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+      <c r="L59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="2">
+        <v>84447</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1146</v>
+      </c>
+      <c r="E60" s="2">
+        <v>14803</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1346</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="3"/>
+        <v>73.688481675392666</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" si="4"/>
+        <v>10.99777117384844</v>
+      </c>
+      <c r="I60" s="3">
+        <f t="shared" si="5"/>
+        <v>0.14914861460957179</v>
+      </c>
+      <c r="J60" t="s">
+        <v>97</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="L60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="2">
+        <v>93338</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1230</v>
+      </c>
+      <c r="E61" s="2">
+        <v>16133</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1457</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="3"/>
+        <v>75.884552845528461</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" si="4"/>
+        <v>11.072752230610844</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="5"/>
+        <v>0.14737236345698862</v>
+      </c>
+      <c r="J61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="2">
+        <v>82313</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1131</v>
+      </c>
+      <c r="E62" s="2">
+        <v>22395</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1363</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="3"/>
+        <v>72.778956675508397</v>
+      </c>
+      <c r="H62" s="1">
+        <f t="shared" si="4"/>
+        <v>16.430667644900954</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="shared" si="5"/>
+        <v>0.21388050578752341</v>
+      </c>
+      <c r="J62" t="s">
+        <v>97</v>
+      </c>
+      <c r="K62">
+        <v>4</v>
+      </c>
+      <c r="L62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="2">
+        <v>89029</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1207</v>
+      </c>
+      <c r="E63" s="2">
+        <v>35180</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1571</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="3"/>
+        <v>73.760563380281695</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" si="4"/>
+        <v>22.393380012730745</v>
+      </c>
+      <c r="I63" s="3">
+        <f t="shared" si="5"/>
+        <v>0.28323229395615457</v>
+      </c>
+      <c r="J63" t="s">
+        <v>97</v>
+      </c>
+      <c r="K63">
+        <v>4</v>
+      </c>
+      <c r="L63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="2">
+        <v>92001</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1175</v>
+      </c>
+      <c r="E64" s="2">
+        <v>23881</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1327</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="3"/>
+        <v>78.298723404255313</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="4"/>
+        <v>17.996232102486811</v>
+      </c>
+      <c r="I64" s="3">
+        <f t="shared" si="5"/>
+        <v>0.20608032308727844</v>
+      </c>
+      <c r="J64" t="s">
+        <v>97</v>
+      </c>
+      <c r="K64">
+        <v>4</v>
+      </c>
+      <c r="L64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="2">
+        <v>95143</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1206</v>
+      </c>
+      <c r="E65" s="2">
+        <v>35261</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1446</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="3"/>
+        <v>78.891376451077946</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="4"/>
+        <v>24.385200553250346</v>
+      </c>
+      <c r="I65" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27039814729609524</v>
+      </c>
+      <c r="J65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="2">
+        <v>100626</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1226</v>
+      </c>
+      <c r="E66" s="2">
+        <v>19378</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1413</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="3"/>
+        <v>82.076672104404565</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" si="4"/>
+        <v>13.714083510261855</v>
+      </c>
+      <c r="I66" s="3">
+        <f t="shared" si="5"/>
+        <v>0.16147795073497551</v>
+      </c>
+      <c r="J66" t="s">
+        <v>82</v>
+      </c>
+      <c r="K66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="2">
+        <v>109308</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1276</v>
+      </c>
+      <c r="E67" s="2">
+        <v>17003</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1482</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="3"/>
+        <v>85.664576802507838</v>
+      </c>
+      <c r="H67" s="1">
+        <f t="shared" si="4"/>
+        <v>11.473009446693657</v>
+      </c>
+      <c r="I67" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13461218737877145</v>
+      </c>
+      <c r="J67" t="s">
+        <v>82</v>
+      </c>
+      <c r="K67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="2">
+        <v>107972</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1261</v>
+      </c>
+      <c r="E68" s="2">
+        <v>22796</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1457</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="3"/>
+        <v>85.624107850911969</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="shared" si="4"/>
+        <v>15.645847632120796</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="5"/>
+        <v>0.17432399363758719</v>
+      </c>
+      <c r="J68" t="s">
+        <v>82</v>
+      </c>
+      <c r="K68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="2">
+        <v>104605</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1235</v>
+      </c>
+      <c r="E69" s="2">
+        <v>29748</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1429</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="3"/>
+        <v>84.700404858299592</v>
+      </c>
+      <c r="H69" s="1">
+        <f t="shared" si="4"/>
+        <v>20.817354793561933</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="5"/>
+        <v>0.2214167156669371</v>
+      </c>
+      <c r="J69" t="s">
+        <v>82</v>
+      </c>
+      <c r="K69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="2">
+        <v>102297</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1246</v>
+      </c>
+      <c r="E70" s="2">
+        <v>34946</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1490</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="3"/>
+        <v>82.100321027287322</v>
+      </c>
+      <c r="H70" s="1">
+        <f t="shared" si="4"/>
+        <v>23.453691275167785</v>
+      </c>
+      <c r="I70" s="3">
+        <f t="shared" si="5"/>
+        <v>0.25462865137019741</v>
+      </c>
+      <c r="J70" t="s">
+        <v>82</v>
+      </c>
+      <c r="K70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="2">
+        <v>106230</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1264</v>
+      </c>
+      <c r="E71" s="2">
+        <v>29036</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1452</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="3"/>
+        <v>84.042721518987335</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" si="4"/>
+        <v>19.997245179063359</v>
+      </c>
+      <c r="I71" s="3">
+        <f t="shared" si="5"/>
+        <v>0.21465852468469535</v>
+      </c>
+      <c r="J71" t="s">
+        <v>81</v>
+      </c>
+      <c r="K71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="2">
+        <v>111440</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1267</v>
+      </c>
+      <c r="E72" s="2">
+        <v>32925</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1449</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="3"/>
+        <v>87.95580110497238</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="4"/>
+        <v>22.722567287784678</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="5"/>
+        <v>0.2280677449520313</v>
+      </c>
+      <c r="J72" t="s">
+        <v>81</v>
+      </c>
+      <c r="K72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="2">
+        <v>106033</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1256</v>
+      </c>
+      <c r="E73" s="2">
+        <v>39710</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1519</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="3"/>
+        <v>84.421178343949038</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="4"/>
+        <v>26.142198815009873</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27246591603027248</v>
+      </c>
+      <c r="J73" t="s">
+        <v>82</v>
+      </c>
+      <c r="K73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="2">
+        <v>110869</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1271</v>
+      </c>
+      <c r="E74" s="2">
+        <v>30191</v>
+      </c>
+      <c r="F74" s="2">
+        <v>1435</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="3"/>
+        <v>87.229740361919752</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="4"/>
+        <v>21.039024390243902</v>
+      </c>
+      <c r="I74" s="3">
+        <f t="shared" si="5"/>
+        <v>0.21402949099673899</v>
+      </c>
+      <c r="J74" t="s">
+        <v>82</v>
+      </c>
+      <c r="K74" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" s="2">
+        <v>48577</v>
+      </c>
+      <c r="D75" s="2">
+        <v>873</v>
+      </c>
+      <c r="E75" s="2">
+        <v>10319</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1038</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="3"/>
+        <v>55.643757159221074</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="4"/>
+        <v>9.9412331406551058</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="5"/>
+        <v>0.17520714479760935</v>
+      </c>
+      <c r="J75" t="s">
+        <v>94</v>
+      </c>
+      <c r="K75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C76" s="2">
+        <v>50915</v>
+      </c>
+      <c r="D76" s="2">
+        <v>886</v>
+      </c>
+      <c r="E76" s="2">
+        <v>12660</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1027</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="3"/>
+        <v>57.466139954853276</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="4"/>
+        <v>12.327166504381694</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="5"/>
+        <v>0.19913488006291782</v>
+      </c>
+      <c r="J76" t="s">
+        <v>94</v>
+      </c>
+      <c r="K76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="2">
+        <v>37003</v>
+      </c>
+      <c r="D77" s="2">
+        <v>790</v>
+      </c>
+      <c r="E77" s="2">
+        <v>11505</v>
+      </c>
+      <c r="F77" s="2">
+        <v>866</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="3"/>
+        <v>46.839240506329112</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="4"/>
+        <v>13.285219399538105</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23717737280448586</v>
+      </c>
+      <c r="J77" t="s">
+        <v>94</v>
+      </c>
+      <c r="K77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="2">
+        <v>62382</v>
+      </c>
+      <c r="D78" s="2">
+        <v>981</v>
+      </c>
+      <c r="E78" s="2">
+        <v>14257</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1133</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="3"/>
+        <v>63.590214067278289</v>
+      </c>
+      <c r="H78" s="1">
+        <f t="shared" si="4"/>
+        <v>12.583406884377759</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1860280014092042</v>
+      </c>
+      <c r="J78" t="s">
+        <v>94</v>
+      </c>
+      <c r="K78" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="2">
+        <v>103396</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1247</v>
+      </c>
+      <c r="E79" s="2">
+        <v>32158</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1450</v>
+      </c>
+      <c r="G79" s="1">
+        <f t="shared" si="3"/>
+        <v>82.915797914995991</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" si="4"/>
+        <v>22.177931034482757</v>
+      </c>
+      <c r="I79" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23723386989686768</v>
+      </c>
+      <c r="J79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="2">
+        <v>99489</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1238</v>
+      </c>
+      <c r="E80" s="2">
+        <v>28640</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1425</v>
+      </c>
+      <c r="G80" s="1">
+        <f t="shared" si="3"/>
+        <v>80.362681744749594</v>
+      </c>
+      <c r="H80" s="1">
+        <f t="shared" si="4"/>
+        <v>20.098245614035086</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="5"/>
+        <v>0.22352472898407075</v>
+      </c>
+      <c r="J80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" s="2">
+        <v>123714</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1407</v>
+      </c>
+      <c r="E81" s="2">
+        <v>46399</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1628</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" si="3"/>
+        <v>87.927505330490405</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" si="4"/>
+        <v>28.500614250614252</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27275399293410851</v>
+      </c>
+      <c r="J81" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" s="2">
+        <v>81521</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1143</v>
+      </c>
+      <c r="E82" s="2">
+        <v>14823</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1338</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="3"/>
+        <v>71.321959755030619</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="4"/>
+        <v>11.078475336322869</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="5"/>
+        <v>0.15385493647762186</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+      <c r="C83" s="2">
+        <v>93657</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1210</v>
+      </c>
+      <c r="E83" s="2">
+        <v>44894</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1620</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="3"/>
+        <v>77.40247933884298</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="4"/>
+        <v>27.712345679012344</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="5"/>
+        <v>0.32402508823465725</v>
+      </c>
+      <c r="J83" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84" s="2">
+        <v>39901</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1039</v>
+      </c>
+      <c r="E84" s="2">
+        <v>23195</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1296</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="3"/>
+        <v>38.403272377285852</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="4"/>
+        <v>17.897376543209877</v>
+      </c>
+      <c r="I84" s="3">
+        <f t="shared" si="5"/>
+        <v>0.36761442880689743</v>
+      </c>
+      <c r="J84" t="s">
+        <v>94</v>
+      </c>
+      <c r="K84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="2">
+        <v>43794</v>
+      </c>
+      <c r="D85" s="2">
+        <v>822</v>
+      </c>
+      <c r="E85" s="2">
+        <v>8433</v>
+      </c>
+      <c r="F85" s="2">
+        <v>989</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="3"/>
+        <v>53.277372262773724</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="4"/>
+        <v>8.5267947421638013</v>
+      </c>
+      <c r="I85" s="3">
+        <f t="shared" si="5"/>
+        <v>0.16146820610029294</v>
+      </c>
+      <c r="J85" t="s">
+        <v>94</v>
+      </c>
+      <c r="K85" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="2">
+        <v>98025</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1220</v>
+      </c>
+      <c r="E86" s="2">
+        <v>34450</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1453</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="3"/>
+        <v>80.348360655737707</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="4"/>
+        <v>23.709566414315209</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" si="5"/>
+        <v>0.2600490658614833</v>
+      </c>
+      <c r="J86" t="s">
+        <v>97</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="2">
+        <v>82261</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1126</v>
+      </c>
+      <c r="E87" s="2">
+        <v>27018</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1393</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="3"/>
+        <v>73.055950266429846</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="4"/>
+        <v>19.395549174443648</v>
+      </c>
+      <c r="I87" s="3">
+        <f t="shared" si="5"/>
+        <v>0.24723871924157431</v>
+      </c>
+      <c r="J87" t="s">
+        <v>97</v>
+      </c>
+      <c r="K87">
+        <v>2</v>
+      </c>
+      <c r="L87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="2">
+        <v>91385</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1201</v>
+      </c>
+      <c r="E88" s="2">
+        <v>16991</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1376</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="3"/>
+        <v>76.090757701915066</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="4"/>
+        <v>12.34811046511628</v>
+      </c>
+      <c r="I88" s="3">
+        <f t="shared" si="5"/>
+        <v>0.15677825348785709</v>
+      </c>
+      <c r="J88" t="s">
+        <v>97</v>
+      </c>
+      <c r="K88">
+        <v>2</v>
+      </c>
+      <c r="L88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="2">
+        <v>91435</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1182</v>
+      </c>
+      <c r="E89" s="2">
+        <v>33613</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1419</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="3"/>
+        <v>77.356175972927247</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="4"/>
+        <v>23.687808315715291</v>
+      </c>
+      <c r="I89" s="3">
+        <f t="shared" si="5"/>
+        <v>0.26880078050028788</v>
+      </c>
+      <c r="J89" t="s">
+        <v>97</v>
+      </c>
+      <c r="K89">
+        <v>2</v>
+      </c>
+      <c r="L89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" s="2">
+        <v>99038</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1228</v>
+      </c>
+      <c r="E90" s="2">
+        <v>29008</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1485</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="3"/>
+        <v>80.649837133550491</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="4"/>
+        <v>19.534006734006734</v>
+      </c>
+      <c r="I90" s="3">
+        <f t="shared" si="5"/>
+        <v>0.22654358589881762</v>
+      </c>
+      <c r="J90" t="s">
+        <v>97</v>
+      </c>
+      <c r="K90">
+        <v>2</v>
+      </c>
+      <c r="L90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="2">
+        <v>88027</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1194</v>
+      </c>
+      <c r="E91" s="2">
+        <v>32674</v>
+      </c>
+      <c r="F91" s="2">
+        <v>1503</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="3"/>
+        <v>73.724455611390283</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="4"/>
+        <v>21.739188290086492</v>
+      </c>
+      <c r="I91" s="3">
+        <f t="shared" si="5"/>
+        <v>0.27070198258506556</v>
+      </c>
+      <c r="J91" t="s">
+        <v>97</v>
+      </c>
+      <c r="K91">
+        <v>2</v>
+      </c>
+      <c r="L91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="2">
+        <v>87078</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1158</v>
+      </c>
+      <c r="E92" s="2">
+        <v>31431</v>
+      </c>
+      <c r="F92" s="2">
+        <v>1431</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="3"/>
+        <v>75.196891191709838</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" si="4"/>
+        <v>21.964360587002098</v>
+      </c>
+      <c r="I92" s="3">
+        <f t="shared" si="5"/>
+        <v>0.26522036301040425</v>
+      </c>
+      <c r="J92" t="s">
+        <v>97</v>
+      </c>
+      <c r="K92">
+        <v>2</v>
+      </c>
+      <c r="L92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="2">
+        <v>31081</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1186</v>
+      </c>
+      <c r="E93" s="2">
+        <v>25148</v>
+      </c>
+      <c r="F93" s="2">
+        <v>1383</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="3"/>
+        <v>26.206576728499158</v>
+      </c>
+      <c r="H93" s="1">
+        <f t="shared" si="4"/>
+        <v>18.183658712942879</v>
+      </c>
+      <c r="I93" s="3">
+        <f t="shared" si="5"/>
+        <v>0.44724252609863235</v>
+      </c>
+      <c r="J93" t="s">
+        <v>97</v>
+      </c>
+      <c r="K93">
+        <v>2</v>
+      </c>
+      <c r="L93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="2">
+        <v>94029</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1211</v>
+      </c>
+      <c r="E94" s="2">
+        <v>28865</v>
+      </c>
+      <c r="F94" s="2">
+        <v>1447</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="3"/>
+        <v>77.645747316267546</v>
+      </c>
+      <c r="H94" s="1">
+        <f t="shared" si="4"/>
+        <v>19.948168624740845</v>
+      </c>
+      <c r="I94" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23487721125522809</v>
+      </c>
+      <c r="J94" t="s">
+        <v>97</v>
+      </c>
+      <c r="K94">
+        <v>2</v>
+      </c>
+      <c r="L94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>108</v>
+      </c>
+      <c r="J95" t="s">
+        <v>97</v>
+      </c>
+      <c r="K95">
+        <v>2</v>
+      </c>
+      <c r="L95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>117</v>
+      </c>
+      <c r="K96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>118</v>
+      </c>
+      <c r="K97">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
manual sheet now has all regional sites
</commit_message>
<xml_diff>
--- a/data/google_earth_manual.xlsx
+++ b/data/google_earth_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\BB_parks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8855999-F132-422A-A29D-7B300E30E153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274104CF-7847-45C5-BBAE-67311F27B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{810870C9-568A-4025-AECC-CEADD1B80506}"/>
+    <workbookView xWindow="-20490" yWindow="990" windowWidth="18900" windowHeight="11025" xr2:uid="{810870C9-568A-4025-AECC-CEADD1B80506}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="207">
   <si>
     <t>Detroit Western</t>
   </si>
@@ -392,6 +392,270 @@
   </si>
   <si>
     <t>Pewamo Westphalia</t>
+  </si>
+  <si>
+    <t>YE_2022_rank</t>
+  </si>
+  <si>
+    <t>Conf</t>
+  </si>
+  <si>
+    <t>Conf_level</t>
+  </si>
+  <si>
+    <t>CAAC</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>***** REGIONAL HOSTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borden Field  Coldwater </t>
+  </si>
+  <si>
+    <t>Mt Pleasant High School</t>
+  </si>
+  <si>
+    <t>Novi High School</t>
+  </si>
+  <si>
+    <t>West Bloomfield High School</t>
+  </si>
+  <si>
+    <t>Rochester High School</t>
+  </si>
+  <si>
+    <t>Joe Pitack Field Klenk Park — Alma Scots Baseball Field</t>
+  </si>
+  <si>
+    <t>Cornerstone Baseball Field - Grand Rapids</t>
+  </si>
+  <si>
+    <t>Jenison High School</t>
+  </si>
+  <si>
+    <t>Portage Northern High School</t>
+  </si>
+  <si>
+    <t>Saginaw heritage high School</t>
+  </si>
+  <si>
+    <t>Troy Athens High School</t>
+  </si>
+  <si>
+    <t>Gross Point North High School</t>
+  </si>
+  <si>
+    <t>Stevenson High School</t>
+  </si>
+  <si>
+    <t>James Gulliver Field - Allen Park</t>
+  </si>
+  <si>
+    <t>Lincoln Baseball - Ypsi</t>
+  </si>
+  <si>
+    <t>Trenton</t>
+  </si>
+  <si>
+    <t>Borden Field  Coldwater</t>
+  </si>
+  <si>
+    <t>Clarenceville High School - Livonia (Stadium</t>
+  </si>
+  <si>
+    <t>Airport High School - Carleton (Varsity Baseball Field)</t>
+  </si>
+  <si>
+    <t>Livonia Franklin</t>
+  </si>
+  <si>
+    <t>Edwardsburg Baseball Field</t>
+  </si>
+  <si>
+    <t>Gainey Athletic Complex - Baseball - Grand Rapids</t>
+  </si>
+  <si>
+    <t>Hope College - Holland</t>
+  </si>
+  <si>
+    <t>Eaton Rapids High School</t>
+  </si>
+  <si>
+    <t>Turcott Field - Petoskey</t>
+  </si>
+  <si>
+    <t>Ionia</t>
+  </si>
+  <si>
+    <t>John C. Huizenga Field - Whitehall</t>
+  </si>
+  <si>
+    <t>Wilmot Field (Wilmot) - Gladwin</t>
+  </si>
+  <si>
+    <t>Clare HS</t>
+  </si>
+  <si>
+    <t>Williamston High School</t>
+  </si>
+  <si>
+    <t>Saginaw Swan Valley</t>
+  </si>
+  <si>
+    <t>Richmond Baseball Facility</t>
+  </si>
+  <si>
+    <t>SVSU (Baseball Diamond)</t>
+  </si>
+  <si>
+    <t>Region Host?</t>
+  </si>
+  <si>
+    <t>Region_div</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Ecorse High School</t>
+  </si>
+  <si>
+    <t>Bad Axe High School</t>
+  </si>
+  <si>
+    <t>Whaley Park - Flint</t>
+  </si>
+  <si>
+    <t>University Liggett School</t>
+  </si>
+  <si>
+    <t>Sanborn Park - Port Huron</t>
+  </si>
+  <si>
+    <t>Davenport University - Grand Rapids</t>
+  </si>
+  <si>
+    <t>Lansing Catholic High School</t>
+  </si>
+  <si>
+    <t>Chesaning Baseball Field</t>
+  </si>
+  <si>
+    <t>Bangor High School - Baseball</t>
+  </si>
+  <si>
+    <t>Centreville High School - Baseball</t>
+  </si>
+  <si>
+    <t>Sand Creek High School - Baseball</t>
+  </si>
+  <si>
+    <t>Lumen Christi Catholic High School</t>
+  </si>
+  <si>
+    <t>Bronson High School - Baseball</t>
+  </si>
+  <si>
+    <t>Adrian College</t>
+  </si>
+  <si>
+    <t>Gladstone Sports Park</t>
+  </si>
+  <si>
+    <t>Standish-Sterling Central High School</t>
+  </si>
+  <si>
+    <t>Mason County Central - Baseball - Scottville</t>
+  </si>
+  <si>
+    <t>Traverse City St Francis</t>
+  </si>
+  <si>
+    <t>Harbor Springs High School</t>
+  </si>
+  <si>
+    <t>Kalamazoo College</t>
+  </si>
+  <si>
+    <t>Camden-Frontier High School</t>
+  </si>
+  <si>
+    <t>Concord Baseball Field</t>
+  </si>
+  <si>
+    <t>Decatur High School - Baseball</t>
+  </si>
+  <si>
+    <t>Lockhart Field - Frankfort</t>
+  </si>
+  <si>
+    <t>Merrill High School</t>
+  </si>
+  <si>
+    <t>Dansville Baseball Field</t>
+  </si>
+  <si>
+    <t>Holton High sChool - Baseball</t>
+  </si>
+  <si>
+    <t>Dow Diamond (Baseball Field)</t>
+  </si>
+  <si>
+    <t>Gabriel Richard HS - Baseball</t>
+  </si>
+  <si>
+    <t>USA Baseball Field - Sebewaing</t>
+  </si>
+  <si>
+    <t>Mayville High School</t>
+  </si>
+  <si>
+    <t>Parkway Christian School - Baseball - Sterling Heights</t>
+  </si>
+  <si>
+    <t>JIMMY JOHN'S STADIUM - Utica</t>
+  </si>
+  <si>
+    <t>Lorenson Field - Ironwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whittemore-Prescott High School </t>
+  </si>
+  <si>
+    <t>Glen Lake High School - Baseball - Maple City</t>
+  </si>
+  <si>
+    <t>Pioneer Park - Baseball - Pellston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudyard </t>
+  </si>
+  <si>
+    <t>high schoo</t>
+  </si>
+  <si>
+    <t>Centennial Field - Beverly Hills - (DETROIT COUNTRY DAAY?)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Wayne State University - Harwell Field</t>
+  </si>
+  <si>
+    <t>Holland Christian High School</t>
+  </si>
+  <si>
+    <t>Holland Christian - Maroons Field - Holland</t>
   </si>
 </sst>
 </file>
@@ -759,26 +1023,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995A9B2-ED22-410A-BC8E-AC27A4E2E923}">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:Q175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q121" sqref="Q121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -809,8 +1074,23 @@
       <c r="K1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -847,8 +1127,14 @@
       <c r="K2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -885,8 +1171,14 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -923,8 +1215,14 @@
       <c r="K4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -964,8 +1262,14 @@
       <c r="L5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1002,8 +1306,14 @@
       <c r="K6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1040,8 +1350,14 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1078,8 +1394,14 @@
       <c r="K8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1116,8 +1438,14 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1154,8 +1482,14 @@
       <c r="K10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1192,8 +1526,14 @@
       <c r="K11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1230,8 +1570,14 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1268,8 +1614,14 @@
       <c r="K13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>122</v>
+      </c>
+      <c r="N13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1306,8 +1658,14 @@
       <c r="K14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1344,8 +1702,14 @@
       <c r="K15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1382,8 +1746,14 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>122</v>
+      </c>
+      <c r="N16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1421,7 +1791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1458,8 +1828,14 @@
       <c r="K18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1496,8 +1872,14 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1532,7 +1914,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1569,8 +1951,14 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>122</v>
+      </c>
+      <c r="N21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1608,7 +1996,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1646,7 +2034,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1683,8 +2071,14 @@
       <c r="K24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>122</v>
+      </c>
+      <c r="N24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1721,8 +2115,14 @@
       <c r="K25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>122</v>
+      </c>
+      <c r="N25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1756,8 +2156,14 @@
       <c r="J26" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>122</v>
+      </c>
+      <c r="N26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1795,7 +2201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1833,7 +2239,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1871,7 +2277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1912,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1953,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4281,16 +4687,1063 @@
       <c r="B96" t="s">
         <v>117</v>
       </c>
+      <c r="J96" t="s">
+        <v>97</v>
+      </c>
       <c r="K96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>118</v>
       </c>
+      <c r="J97" t="s">
+        <v>97</v>
+      </c>
       <c r="K97">
         <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>127</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="O99" t="s">
+        <v>162</v>
+      </c>
+      <c r="P99">
+        <v>1</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>204</v>
+      </c>
+      <c r="J100" t="s">
+        <v>82</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="O100" t="s">
+        <v>162</v>
+      </c>
+      <c r="P100">
+        <v>1</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>128</v>
+      </c>
+      <c r="J101" t="s">
+        <v>201</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="O101" t="s">
+        <v>162</v>
+      </c>
+      <c r="P101">
+        <v>1</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>129</v>
+      </c>
+      <c r="J102" t="s">
+        <v>97</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="O102" t="s">
+        <v>162</v>
+      </c>
+      <c r="P102">
+        <v>1</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>130</v>
+      </c>
+      <c r="J103" t="s">
+        <v>97</v>
+      </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="O103" t="s">
+        <v>162</v>
+      </c>
+      <c r="P103">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>131</v>
+      </c>
+      <c r="J104" t="s">
+        <v>97</v>
+      </c>
+      <c r="O104" t="s">
+        <v>162</v>
+      </c>
+      <c r="P104">
+        <v>1</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>132</v>
+      </c>
+      <c r="J105" t="s">
+        <v>82</v>
+      </c>
+      <c r="O105" t="s">
+        <v>162</v>
+      </c>
+      <c r="P105">
+        <v>1</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="J106" t="s">
+        <v>82</v>
+      </c>
+      <c r="O106" t="s">
+        <v>162</v>
+      </c>
+      <c r="P106">
+        <v>1</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>134</v>
+      </c>
+      <c r="J107" t="s">
+        <v>97</v>
+      </c>
+      <c r="O107" t="s">
+        <v>162</v>
+      </c>
+      <c r="P107">
+        <v>1</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>135</v>
+      </c>
+      <c r="J108" t="s">
+        <v>97</v>
+      </c>
+      <c r="O108" t="s">
+        <v>162</v>
+      </c>
+      <c r="P108">
+        <v>1</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>136</v>
+      </c>
+      <c r="O109" t="s">
+        <v>162</v>
+      </c>
+      <c r="P109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>137</v>
+      </c>
+      <c r="O110" t="s">
+        <v>162</v>
+      </c>
+      <c r="P110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>138</v>
+      </c>
+      <c r="O111" t="s">
+        <v>162</v>
+      </c>
+      <c r="P111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>139</v>
+      </c>
+      <c r="O112" t="s">
+        <v>162</v>
+      </c>
+      <c r="P112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>140</v>
+      </c>
+      <c r="O113" t="s">
+        <v>162</v>
+      </c>
+      <c r="P113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>141</v>
+      </c>
+      <c r="O114" t="s">
+        <v>162</v>
+      </c>
+      <c r="P114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>73</v>
+      </c>
+      <c r="J115" t="s">
+        <v>82</v>
+      </c>
+      <c r="O115" t="s">
+        <v>162</v>
+      </c>
+      <c r="P115">
+        <v>2</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>142</v>
+      </c>
+      <c r="J116" t="s">
+        <v>97</v>
+      </c>
+      <c r="O116" t="s">
+        <v>162</v>
+      </c>
+      <c r="P116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>143</v>
+      </c>
+      <c r="O117" t="s">
+        <v>162</v>
+      </c>
+      <c r="P117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>144</v>
+      </c>
+      <c r="J118" t="s">
+        <v>97</v>
+      </c>
+      <c r="O118" t="s">
+        <v>162</v>
+      </c>
+      <c r="P118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>145</v>
+      </c>
+      <c r="J119" t="s">
+        <v>97</v>
+      </c>
+      <c r="O119" t="s">
+        <v>162</v>
+      </c>
+      <c r="P119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>146</v>
+      </c>
+      <c r="O120" t="s">
+        <v>162</v>
+      </c>
+      <c r="P120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>206</v>
+      </c>
+      <c r="O121" t="s">
+        <v>162</v>
+      </c>
+      <c r="P121">
+        <v>2</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>147</v>
+      </c>
+      <c r="O122" t="s">
+        <v>162</v>
+      </c>
+      <c r="P122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>148</v>
+      </c>
+      <c r="O123" t="s">
+        <v>162</v>
+      </c>
+      <c r="P123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>149</v>
+      </c>
+      <c r="J124" t="s">
+        <v>82</v>
+      </c>
+      <c r="O124" t="s">
+        <v>162</v>
+      </c>
+      <c r="P124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>150</v>
+      </c>
+      <c r="J125" t="s">
+        <v>97</v>
+      </c>
+      <c r="O125" t="s">
+        <v>162</v>
+      </c>
+      <c r="P125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>151</v>
+      </c>
+      <c r="O126" t="s">
+        <v>162</v>
+      </c>
+      <c r="P126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>152</v>
+      </c>
+      <c r="J127" t="s">
+        <v>97</v>
+      </c>
+      <c r="O127" t="s">
+        <v>162</v>
+      </c>
+      <c r="P127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>153</v>
+      </c>
+      <c r="O128" t="s">
+        <v>162</v>
+      </c>
+      <c r="P128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>154</v>
+      </c>
+      <c r="O129" t="s">
+        <v>162</v>
+      </c>
+      <c r="P129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>155</v>
+      </c>
+      <c r="J130" t="s">
+        <v>97</v>
+      </c>
+      <c r="O130" t="s">
+        <v>162</v>
+      </c>
+      <c r="P130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>202</v>
+      </c>
+      <c r="O131" t="s">
+        <v>162</v>
+      </c>
+      <c r="P131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>156</v>
+      </c>
+      <c r="J132" t="s">
+        <v>97</v>
+      </c>
+      <c r="O132" t="s">
+        <v>162</v>
+      </c>
+      <c r="P132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>157</v>
+      </c>
+      <c r="O133" t="s">
+        <v>162</v>
+      </c>
+      <c r="P133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>158</v>
+      </c>
+      <c r="O134" t="s">
+        <v>162</v>
+      </c>
+      <c r="P134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>159</v>
+      </c>
+      <c r="J135" t="s">
+        <v>82</v>
+      </c>
+      <c r="O135" t="s">
+        <v>162</v>
+      </c>
+      <c r="P135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>163</v>
+      </c>
+      <c r="J136" t="s">
+        <v>97</v>
+      </c>
+      <c r="O136" t="s">
+        <v>162</v>
+      </c>
+      <c r="P136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>164</v>
+      </c>
+      <c r="J137" t="s">
+        <v>97</v>
+      </c>
+      <c r="O137" t="s">
+        <v>162</v>
+      </c>
+      <c r="P137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>165</v>
+      </c>
+      <c r="O138" t="s">
+        <v>162</v>
+      </c>
+      <c r="P138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>166</v>
+      </c>
+      <c r="J139" t="s">
+        <v>97</v>
+      </c>
+      <c r="O139" t="s">
+        <v>162</v>
+      </c>
+      <c r="P139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>167</v>
+      </c>
+      <c r="O140" t="s">
+        <v>162</v>
+      </c>
+      <c r="P140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>168</v>
+      </c>
+      <c r="J141" t="s">
+        <v>82</v>
+      </c>
+      <c r="O141" t="s">
+        <v>162</v>
+      </c>
+      <c r="P141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>169</v>
+      </c>
+      <c r="J142" t="s">
+        <v>97</v>
+      </c>
+      <c r="O142" t="s">
+        <v>162</v>
+      </c>
+      <c r="P142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>170</v>
+      </c>
+      <c r="O143" t="s">
+        <v>162</v>
+      </c>
+      <c r="P143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>171</v>
+      </c>
+      <c r="J144" t="s">
+        <v>97</v>
+      </c>
+      <c r="O144" t="s">
+        <v>162</v>
+      </c>
+      <c r="P144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>168</v>
+      </c>
+      <c r="J145" t="s">
+        <v>82</v>
+      </c>
+      <c r="O145" t="s">
+        <v>162</v>
+      </c>
+      <c r="P145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>172</v>
+      </c>
+      <c r="J146" t="s">
+        <v>97</v>
+      </c>
+      <c r="O146" t="s">
+        <v>162</v>
+      </c>
+      <c r="P146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>173</v>
+      </c>
+      <c r="J147" t="s">
+        <v>97</v>
+      </c>
+      <c r="O147" t="s">
+        <v>162</v>
+      </c>
+      <c r="P147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>174</v>
+      </c>
+      <c r="J148" t="s">
+        <v>97</v>
+      </c>
+      <c r="O148" t="s">
+        <v>162</v>
+      </c>
+      <c r="P148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>175</v>
+      </c>
+      <c r="J149" t="s">
+        <v>97</v>
+      </c>
+      <c r="O149" t="s">
+        <v>162</v>
+      </c>
+      <c r="P149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>176</v>
+      </c>
+      <c r="J150" t="s">
+        <v>82</v>
+      </c>
+      <c r="O150" t="s">
+        <v>162</v>
+      </c>
+      <c r="P150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>177</v>
+      </c>
+      <c r="O151" t="s">
+        <v>162</v>
+      </c>
+      <c r="P151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>178</v>
+      </c>
+      <c r="J152" t="s">
+        <v>97</v>
+      </c>
+      <c r="O152" t="s">
+        <v>162</v>
+      </c>
+      <c r="P152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>179</v>
+      </c>
+      <c r="J153" t="s">
+        <v>97</v>
+      </c>
+      <c r="O153" t="s">
+        <v>162</v>
+      </c>
+      <c r="P153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>180</v>
+      </c>
+      <c r="J154" t="s">
+        <v>97</v>
+      </c>
+      <c r="O154" t="s">
+        <v>162</v>
+      </c>
+      <c r="P154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>181</v>
+      </c>
+      <c r="J155" t="s">
+        <v>97</v>
+      </c>
+      <c r="O155" t="s">
+        <v>162</v>
+      </c>
+      <c r="P155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>182</v>
+      </c>
+      <c r="J156" t="s">
+        <v>82</v>
+      </c>
+      <c r="O156" t="s">
+        <v>162</v>
+      </c>
+      <c r="P156">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>183</v>
+      </c>
+      <c r="J157" t="s">
+        <v>97</v>
+      </c>
+      <c r="O157" t="s">
+        <v>162</v>
+      </c>
+      <c r="P157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>184</v>
+      </c>
+      <c r="O158" t="s">
+        <v>162</v>
+      </c>
+      <c r="P158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>185</v>
+      </c>
+      <c r="J159" t="s">
+        <v>97</v>
+      </c>
+      <c r="O159" t="s">
+        <v>162</v>
+      </c>
+      <c r="P159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>186</v>
+      </c>
+      <c r="O160" t="s">
+        <v>162</v>
+      </c>
+      <c r="P160">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>187</v>
+      </c>
+      <c r="J161" t="s">
+        <v>97</v>
+      </c>
+      <c r="O161" t="s">
+        <v>162</v>
+      </c>
+      <c r="P161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>188</v>
+      </c>
+      <c r="J162" t="s">
+        <v>97</v>
+      </c>
+      <c r="O162" t="s">
+        <v>162</v>
+      </c>
+      <c r="P162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>189</v>
+      </c>
+      <c r="J163" t="s">
+        <v>97</v>
+      </c>
+      <c r="O163" t="s">
+        <v>162</v>
+      </c>
+      <c r="P163">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>190</v>
+      </c>
+      <c r="J164" t="s">
+        <v>81</v>
+      </c>
+      <c r="O164" t="s">
+        <v>162</v>
+      </c>
+      <c r="P164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>191</v>
+      </c>
+      <c r="J165" t="s">
+        <v>97</v>
+      </c>
+      <c r="O165" t="s">
+        <v>162</v>
+      </c>
+      <c r="P165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>192</v>
+      </c>
+      <c r="O166" t="s">
+        <v>162</v>
+      </c>
+      <c r="P166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>193</v>
+      </c>
+      <c r="J167" t="s">
+        <v>97</v>
+      </c>
+      <c r="O167" t="s">
+        <v>162</v>
+      </c>
+      <c r="P167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>194</v>
+      </c>
+      <c r="O168" t="s">
+        <v>162</v>
+      </c>
+      <c r="P168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>195</v>
+      </c>
+      <c r="O169" t="s">
+        <v>162</v>
+      </c>
+      <c r="P169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>196</v>
+      </c>
+      <c r="O170" t="s">
+        <v>162</v>
+      </c>
+      <c r="P170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>197</v>
+      </c>
+      <c r="J171" t="s">
+        <v>97</v>
+      </c>
+      <c r="O171" t="s">
+        <v>162</v>
+      </c>
+      <c r="P171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>198</v>
+      </c>
+      <c r="J172" t="s">
+        <v>97</v>
+      </c>
+      <c r="O172" t="s">
+        <v>162</v>
+      </c>
+      <c r="P172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>199</v>
+      </c>
+      <c r="O173" t="s">
+        <v>162</v>
+      </c>
+      <c r="P173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>200</v>
+      </c>
+      <c r="J174" t="s">
+        <v>97</v>
+      </c>
+      <c r="O174" t="s">
+        <v>162</v>
+      </c>
+      <c r="P174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>205</v>
+      </c>
+      <c r="J175" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4329,5 +5782,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
weds 12-7 end of nigh desktop
</commit_message>
<xml_diff>
--- a/data/google_earth_manual.xlsx
+++ b/data/google_earth_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\BB_parks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2141D554-FD53-48C0-A1A9-F2223ADDCADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C112280E-42F4-486F-9433-36FA214E06B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="265">
   <si>
     <t>School</t>
   </si>
@@ -1219,8 +1219,8 @@
   <dimension ref="A1:Q229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K221" sqref="K221"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J221" sqref="J221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,15 +1307,15 @@
         <v>1462</v>
       </c>
       <c r="G2" s="2">
-        <f>C2/D2</f>
+        <f t="shared" ref="G2:G9" si="0">C2/D2</f>
         <v>84.348106365833999</v>
       </c>
       <c r="H2" s="2">
-        <f>E2/F2</f>
+        <f t="shared" ref="H2:H9" si="1">E2/F2</f>
         <v>22.550615595075239</v>
       </c>
       <c r="I2" s="3">
-        <f>E2/(E2+C2)</f>
+        <f t="shared" ref="I2:I9" si="2">E2/(E2+C2)</f>
         <v>0.23952195866177486</v>
       </c>
       <c r="J2" t="s">
@@ -1345,15 +1345,15 @@
         <v>1413</v>
       </c>
       <c r="G3" s="2">
-        <f>C3/D3</f>
+        <f t="shared" si="0"/>
         <v>82.076672104404565</v>
       </c>
       <c r="H3" s="2">
-        <f>E3/F3</f>
+        <f t="shared" si="1"/>
         <v>13.714083510261855</v>
       </c>
       <c r="I3" s="3">
-        <f>E3/(E3+C3)</f>
+        <f t="shared" si="2"/>
         <v>0.16147795073497551</v>
       </c>
       <c r="J3" t="s">
@@ -1383,15 +1383,15 @@
         <v>1482</v>
       </c>
       <c r="G4" s="2">
-        <f>C4/D4</f>
+        <f t="shared" si="0"/>
         <v>85.664576802507838</v>
       </c>
       <c r="H4" s="2">
-        <f>E4/F4</f>
+        <f t="shared" si="1"/>
         <v>11.473009446693657</v>
       </c>
       <c r="I4" s="3">
-        <f>E4/(E4+C4)</f>
+        <f t="shared" si="2"/>
         <v>0.13461218737877145</v>
       </c>
       <c r="J4" t="s">
@@ -1427,15 +1427,15 @@
         <v>1457</v>
       </c>
       <c r="G5" s="2">
-        <f>C5/D5</f>
+        <f t="shared" si="0"/>
         <v>85.624107850911969</v>
       </c>
       <c r="H5" s="2">
-        <f>E5/F5</f>
+        <f t="shared" si="1"/>
         <v>15.645847632120796</v>
       </c>
       <c r="I5" s="3">
-        <f>E5/(E5+C5)</f>
+        <f t="shared" si="2"/>
         <v>0.17432399363758719</v>
       </c>
       <c r="J5" t="s">
@@ -1465,15 +1465,15 @@
         <v>1429</v>
       </c>
       <c r="G6" s="2">
-        <f>C6/D6</f>
+        <f t="shared" si="0"/>
         <v>84.700404858299592</v>
       </c>
       <c r="H6" s="2">
-        <f>E6/F6</f>
+        <f t="shared" si="1"/>
         <v>20.817354793561933</v>
       </c>
       <c r="I6" s="3">
-        <f>E6/(E6+C6)</f>
+        <f t="shared" si="2"/>
         <v>0.2214167156669371</v>
       </c>
       <c r="J6" t="s">
@@ -1503,15 +1503,15 @@
         <v>1490</v>
       </c>
       <c r="G7" s="2">
-        <f>C7/D7</f>
+        <f t="shared" si="0"/>
         <v>82.100321027287322</v>
       </c>
       <c r="H7" s="2">
-        <f>E7/F7</f>
+        <f t="shared" si="1"/>
         <v>23.453691275167785</v>
       </c>
       <c r="I7" s="3">
-        <f>E7/(E7+C7)</f>
+        <f t="shared" si="2"/>
         <v>0.25462865137019741</v>
       </c>
       <c r="J7" t="s">
@@ -1538,15 +1538,15 @@
         <v>1519</v>
       </c>
       <c r="G8" s="2">
-        <f>C8/D8</f>
+        <f t="shared" si="0"/>
         <v>84.421178343949038</v>
       </c>
       <c r="H8" s="2">
-        <f>E8/F8</f>
+        <f t="shared" si="1"/>
         <v>26.142198815009873</v>
       </c>
       <c r="I8" s="3">
-        <f>E8/(E8+C8)</f>
+        <f t="shared" si="2"/>
         <v>0.27246591603027248</v>
       </c>
       <c r="J8" t="s">
@@ -1579,15 +1579,15 @@
         <v>1435</v>
       </c>
       <c r="G9" s="2">
-        <f>C9/D9</f>
+        <f t="shared" si="0"/>
         <v>87.229740361919752</v>
       </c>
       <c r="H9" s="2">
-        <f>E9/F9</f>
+        <f t="shared" si="1"/>
         <v>21.039024390243902</v>
       </c>
       <c r="I9" s="3">
-        <f>E9/(E9+C9)</f>
+        <f t="shared" si="2"/>
         <v>0.21402949099673899</v>
       </c>
       <c r="J9" t="s">
@@ -1930,15 +1930,15 @@
         <v>1438</v>
       </c>
       <c r="G21" s="2">
-        <f>C21/D21</f>
+        <f t="shared" ref="G21:G52" si="3">C21/D21</f>
         <v>72.259323503902863</v>
       </c>
       <c r="H21" s="2">
-        <f>E21/F21</f>
+        <f t="shared" ref="H21:H52" si="4">E21/F21</f>
         <v>24.755910987482615</v>
       </c>
       <c r="I21" s="3">
-        <f>E21/(E21+C21)</f>
+        <f t="shared" ref="I21:I52" si="5">E21/(E21+C21)</f>
         <v>0.29936761020569486</v>
       </c>
       <c r="J21" t="s">
@@ -1974,15 +1974,15 @@
         <v>1332</v>
       </c>
       <c r="G22" s="2">
-        <f>C22/D22</f>
+        <f t="shared" si="3"/>
         <v>73.918777292576422</v>
       </c>
       <c r="H22" s="2">
-        <f>E22/F22</f>
+        <f t="shared" si="4"/>
         <v>15.311561561561561</v>
       </c>
       <c r="I22" s="3">
-        <f>E22/(E22+C22)</f>
+        <f t="shared" si="5"/>
         <v>0.19417891690151573</v>
       </c>
       <c r="J22" t="s">
@@ -2018,15 +2018,15 @@
         <v>1445</v>
       </c>
       <c r="G23" s="2">
-        <f>C23/D23</f>
+        <f t="shared" si="3"/>
         <v>75.067532467532473</v>
       </c>
       <c r="H23" s="2">
-        <f>E23/F23</f>
+        <f t="shared" si="4"/>
         <v>26.465743944636678</v>
       </c>
       <c r="I23" s="3">
-        <f>E23/(E23+C23)</f>
+        <f t="shared" si="5"/>
         <v>0.30607622492916942</v>
       </c>
       <c r="J23" t="s">
@@ -2062,15 +2062,15 @@
         <v>1417</v>
       </c>
       <c r="G24" s="2">
-        <f>C24/D24</f>
+        <f t="shared" si="3"/>
         <v>83.488046166529273</v>
       </c>
       <c r="H24" s="2">
-        <f>E24/F24</f>
+        <f t="shared" si="4"/>
         <v>26.210303458009879</v>
       </c>
       <c r="I24" s="3">
-        <f>E24/(E24+C24)</f>
+        <f t="shared" si="5"/>
         <v>0.268331274248434</v>
       </c>
       <c r="J24" t="s">
@@ -2115,15 +2115,15 @@
         <v>1598</v>
       </c>
       <c r="G25" s="2">
-        <f>C25/D25</f>
+        <f t="shared" si="3"/>
         <v>77.69916666666667</v>
       </c>
       <c r="H25" s="2">
-        <f>E25/F25</f>
+        <f t="shared" si="4"/>
         <v>23.025031289111389</v>
       </c>
       <c r="I25" s="3">
-        <f>E25/(E25+C25)</f>
+        <f t="shared" si="5"/>
         <v>0.28295894119185128</v>
       </c>
       <c r="J25" t="s">
@@ -2159,15 +2159,15 @@
         <v>1502</v>
       </c>
       <c r="G26" s="2">
-        <f>C26/D26</f>
+        <f t="shared" si="3"/>
         <v>78.542079207920793</v>
       </c>
       <c r="H26" s="2">
-        <f>E26/F26</f>
+        <f t="shared" si="4"/>
         <v>25.449400798934754</v>
       </c>
       <c r="I26" s="3">
-        <f>E26/(E26+C26)</f>
+        <f t="shared" si="5"/>
         <v>0.28650556896370805</v>
       </c>
       <c r="J26" t="s">
@@ -2203,15 +2203,15 @@
         <v>1344</v>
       </c>
       <c r="G27" s="2">
-        <f>C27/D27</f>
+        <f t="shared" si="3"/>
         <v>76.738033072236732</v>
       </c>
       <c r="H27" s="2">
-        <f>E27/F27</f>
+        <f t="shared" si="4"/>
         <v>13.703125</v>
       </c>
       <c r="I27" s="3">
-        <f>E27/(E27+C27)</f>
+        <f t="shared" si="5"/>
         <v>0.17278518421225456</v>
       </c>
       <c r="J27" t="s">
@@ -2253,15 +2253,15 @@
         <v>1428</v>
       </c>
       <c r="G28" s="2">
-        <f>C28/D28</f>
+        <f t="shared" si="3"/>
         <v>80.275313807531376</v>
       </c>
       <c r="H28" s="2">
-        <f>E28/F28</f>
+        <f t="shared" si="4"/>
         <v>25.918067226890756</v>
       </c>
       <c r="I28" s="3">
-        <f>E28/(E28+C28)</f>
+        <f t="shared" si="5"/>
         <v>0.27840379118399278</v>
       </c>
       <c r="J28" t="s">
@@ -2300,15 +2300,15 @@
         <v>1395</v>
       </c>
       <c r="G29" s="2">
-        <f>C29/D29</f>
+        <f t="shared" si="3"/>
         <v>76.185025817555939</v>
       </c>
       <c r="H29" s="2">
-        <f>E29/F29</f>
+        <f t="shared" si="4"/>
         <v>22.187813620071683</v>
       </c>
       <c r="I29" s="3">
-        <f>E29/(E29+C29)</f>
+        <f t="shared" si="5"/>
         <v>0.25905807715163331</v>
       </c>
       <c r="J29" t="s">
@@ -2344,15 +2344,15 @@
         <v>1433</v>
       </c>
       <c r="G30" s="2">
-        <f>C30/D30</f>
+        <f t="shared" si="3"/>
         <v>77.131736526946113</v>
       </c>
       <c r="H30" s="2">
-        <f>E30/F30</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="I30" s="3">
-        <f>E30/(E30+C30)</f>
+        <f t="shared" si="5"/>
         <v>0.2590617373226069</v>
       </c>
       <c r="J30" t="s">
@@ -2394,15 +2394,15 @@
         <v>1431</v>
       </c>
       <c r="G31" s="2">
-        <f>C31/D31</f>
+        <f t="shared" si="3"/>
         <v>79.54038301415487</v>
       </c>
       <c r="H31" s="2">
-        <f>E31/F31</f>
+        <f t="shared" si="4"/>
         <v>17.552061495457721</v>
       </c>
       <c r="I31" s="3">
-        <f>E31/(E31+C31)</f>
+        <f t="shared" si="5"/>
         <v>0.20818931576111732</v>
       </c>
       <c r="J31" t="s">
@@ -2438,15 +2438,15 @@
         <v>1356</v>
       </c>
       <c r="G32" s="2">
-        <f>C32/D32</f>
+        <f t="shared" si="3"/>
         <v>75.289956331877733</v>
       </c>
       <c r="H32" s="2">
-        <f>E32/F32</f>
+        <f t="shared" si="4"/>
         <v>22.103244837758112</v>
       </c>
       <c r="I32" s="3">
-        <f>E32/(E32+C32)</f>
+        <f t="shared" si="5"/>
         <v>0.25798121863675877</v>
       </c>
       <c r="J32" t="s">
@@ -2482,15 +2482,15 @@
         <v>1433</v>
       </c>
       <c r="G33" s="2">
-        <f>C33/D33</f>
+        <f t="shared" si="3"/>
         <v>76.318259385665527</v>
       </c>
       <c r="H33" s="2">
-        <f>E33/F33</f>
+        <f t="shared" si="4"/>
         <v>19.540823447313329</v>
       </c>
       <c r="I33" s="3">
-        <f>E33/(E33+C33)</f>
+        <f t="shared" si="5"/>
         <v>0.23842243735472171</v>
       </c>
       <c r="J33" t="s">
@@ -2526,15 +2526,15 @@
         <v>1369</v>
       </c>
       <c r="G34" s="2">
-        <f>C34/D34</f>
+        <f t="shared" si="3"/>
         <v>83.096013018714402</v>
       </c>
       <c r="H34" s="2">
-        <f>E34/F34</f>
+        <f t="shared" si="4"/>
         <v>12.559532505478451</v>
       </c>
       <c r="I34" s="3">
-        <f>E34/(E34+C34)</f>
+        <f t="shared" si="5"/>
         <v>0.14410110711621787</v>
       </c>
       <c r="J34" t="s">
@@ -2564,15 +2564,15 @@
         <v>1380</v>
       </c>
       <c r="G35" s="2">
-        <f>C35/D35</f>
+        <f t="shared" si="3"/>
         <v>80.71691792294807</v>
       </c>
       <c r="H35" s="2">
-        <f>E35/F35</f>
+        <f t="shared" si="4"/>
         <v>17.984057971014494</v>
       </c>
       <c r="I35" s="3">
-        <f>E35/(E35+C35)</f>
+        <f t="shared" si="5"/>
         <v>0.2047791144776144</v>
       </c>
       <c r="J35" t="s">
@@ -2608,15 +2608,15 @@
         <v>1341</v>
       </c>
       <c r="G36" s="2">
-        <f>C36/D36</f>
+        <f t="shared" si="3"/>
         <v>69.950530035335689</v>
       </c>
       <c r="H36" s="2">
-        <f>E36/F36</f>
+        <f t="shared" si="4"/>
         <v>21.455630126771066</v>
       </c>
       <c r="I36" s="3">
-        <f>E36/(E36+C36)</f>
+        <f t="shared" si="5"/>
         <v>0.26651598799510912</v>
       </c>
       <c r="J36" t="s">
@@ -2652,15 +2652,15 @@
         <v>1166</v>
       </c>
       <c r="G37" s="2">
-        <f>C37/D37</f>
+        <f t="shared" si="3"/>
         <v>62.560056858564323</v>
       </c>
       <c r="H37" s="2">
-        <f>E37/F37</f>
+        <f t="shared" si="4"/>
         <v>23.6852487135506</v>
       </c>
       <c r="I37" s="3">
-        <f>E37/(E37+C37)</f>
+        <f t="shared" si="5"/>
         <v>0.23882081304750127</v>
       </c>
       <c r="J37" t="s">
@@ -2699,15 +2699,15 @@
         <v>1460</v>
       </c>
       <c r="G38" s="2">
-        <f>C38/D38</f>
+        <f t="shared" si="3"/>
         <v>76.169827586206893</v>
       </c>
       <c r="H38" s="2">
-        <f>E38/F38</f>
+        <f t="shared" si="4"/>
         <v>27.122602739726027</v>
       </c>
       <c r="I38" s="3">
-        <f>E38/(E38+C38)</f>
+        <f t="shared" si="5"/>
         <v>0.3094735690393573</v>
       </c>
       <c r="J38" t="s">
@@ -2743,15 +2743,15 @@
         <v>1393</v>
       </c>
       <c r="G39" s="2">
-        <f>C39/D39</f>
+        <f t="shared" si="3"/>
         <v>76.287813310285216</v>
       </c>
       <c r="H39" s="2">
-        <f>E39/F39</f>
+        <f t="shared" si="4"/>
         <v>21.972720746590092</v>
       </c>
       <c r="I39" s="3">
-        <f>E39/(E39+C39)</f>
+        <f t="shared" si="5"/>
         <v>0.25748487882025356</v>
       </c>
       <c r="J39" t="s">
@@ -2796,15 +2796,15 @@
         <v>1417</v>
       </c>
       <c r="G40" s="2">
-        <f>C40/D40</f>
+        <f t="shared" si="3"/>
         <v>77.971145919208567</v>
       </c>
       <c r="H40" s="2">
-        <f>E40/F40</f>
+        <f t="shared" si="4"/>
         <v>13.958362738179252</v>
       </c>
       <c r="I40" s="3">
-        <f>E40/(E40+C40)</f>
+        <f t="shared" si="5"/>
         <v>0.17295685478934575</v>
       </c>
       <c r="J40" t="s">
@@ -2837,15 +2837,15 @@
         <v>1396</v>
       </c>
       <c r="G41" s="2">
-        <f>C41/D41</f>
+        <f t="shared" si="3"/>
         <v>91.496468926553675</v>
       </c>
       <c r="H41" s="2">
-        <f>E41/F41</f>
+        <f t="shared" si="4"/>
         <v>24.48137535816619</v>
       </c>
       <c r="I41" s="3">
-        <f>E41/(E41+C41)</f>
+        <f t="shared" si="5"/>
         <v>0.20872751702446027</v>
       </c>
       <c r="J41" t="s">
@@ -2875,15 +2875,15 @@
         <v>1369</v>
       </c>
       <c r="G42" s="2">
-        <f>C42/D42</f>
+        <f t="shared" si="3"/>
         <v>72.370567375886523</v>
       </c>
       <c r="H42" s="2">
-        <f>E42/F42</f>
+        <f t="shared" si="4"/>
         <v>21.413440467494521</v>
       </c>
       <c r="I42" s="3">
-        <f>E42/(E42+C42)</f>
+        <f t="shared" si="5"/>
         <v>0.2642204977061533</v>
       </c>
       <c r="J42" t="s">
@@ -2913,15 +2913,15 @@
         <v>1424</v>
       </c>
       <c r="G43" s="2">
-        <f>C43/D43</f>
+        <f t="shared" si="3"/>
         <v>75.66724137931034</v>
       </c>
       <c r="H43" s="2">
-        <f>E43/F43</f>
+        <f t="shared" si="4"/>
         <v>19.192415730337078</v>
       </c>
       <c r="I43" s="3">
-        <f>E43/(E43+C43)</f>
+        <f t="shared" si="5"/>
         <v>0.23743744787322768</v>
       </c>
       <c r="J43" t="s">
@@ -2954,15 +2954,15 @@
         <v>1383</v>
       </c>
       <c r="G44" s="2">
-        <f>C44/D44</f>
+        <f t="shared" si="3"/>
         <v>80.227996647108128</v>
       </c>
       <c r="H44" s="2">
-        <f>E44/F44</f>
+        <f t="shared" si="4"/>
         <v>20.765726681127983</v>
       </c>
       <c r="I44" s="3">
-        <f>E44/(E44+C44)</f>
+        <f t="shared" si="5"/>
         <v>0.23080261349663669</v>
       </c>
       <c r="J44" t="s">
@@ -2995,15 +2995,15 @@
         <v>1425</v>
       </c>
       <c r="G45" s="2">
-        <f>C45/D45</f>
+        <f t="shared" si="3"/>
         <v>76.281986531986533</v>
       </c>
       <c r="H45" s="2">
-        <f>E45/F45</f>
+        <f t="shared" si="4"/>
         <v>22.978947368421053</v>
       </c>
       <c r="I45" s="3">
-        <f>E45/(E45+C45)</f>
+        <f t="shared" si="5"/>
         <v>0.26542539394332404</v>
       </c>
       <c r="J45" t="s">
@@ -3036,15 +3036,15 @@
         <v>1395</v>
       </c>
       <c r="G46" s="2">
-        <f>C46/D46</f>
+        <f t="shared" si="3"/>
         <v>78.338668913226627</v>
       </c>
       <c r="H46" s="2">
-        <f>E46/F46</f>
+        <f t="shared" si="4"/>
         <v>18.969892473118279</v>
       </c>
       <c r="I46" s="3">
-        <f>E46/(E46+C46)</f>
+        <f t="shared" si="5"/>
         <v>0.22153853881507898</v>
       </c>
       <c r="J46" t="s">
@@ -3077,15 +3077,15 @@
         <v>1426</v>
       </c>
       <c r="G47" s="2">
-        <f>C47/D47</f>
+        <f t="shared" si="3"/>
         <v>78.5662447257384</v>
       </c>
       <c r="H47" s="2">
-        <f>E47/F47</f>
+        <f t="shared" si="4"/>
         <v>26.419354838709676</v>
       </c>
       <c r="I47" s="3">
-        <f>E47/(E47+C47)</f>
+        <f t="shared" si="5"/>
         <v>0.28808258459185626</v>
       </c>
       <c r="J47" t="s">
@@ -3118,15 +3118,15 @@
         <v>1439</v>
       </c>
       <c r="G48" s="2">
-        <f>C48/D48</f>
+        <f t="shared" si="3"/>
         <v>78.201511335012597</v>
       </c>
       <c r="H48" s="2">
-        <f>E48/F48</f>
+        <f t="shared" si="4"/>
         <v>20.377345378735232</v>
       </c>
       <c r="I48" s="3">
-        <f>E48/(E48+C48)</f>
+        <f t="shared" si="5"/>
         <v>0.23944766088795616</v>
       </c>
       <c r="J48" t="s">
@@ -3159,15 +3159,15 @@
         <v>1402</v>
       </c>
       <c r="G49" s="2">
-        <f>C49/D49</f>
+        <f t="shared" si="3"/>
         <v>76.867634500426988</v>
       </c>
       <c r="H49" s="2">
-        <f>E49/F49</f>
+        <f t="shared" si="4"/>
         <v>23.45506419400856</v>
       </c>
       <c r="I49" s="3">
-        <f>E49/(E49+C49)</f>
+        <f t="shared" si="5"/>
         <v>0.26757583647962507</v>
       </c>
       <c r="J49" t="s">
@@ -3200,15 +3200,15 @@
         <v>1449</v>
       </c>
       <c r="G50" s="2">
-        <f>C50/D50</f>
+        <f t="shared" si="3"/>
         <v>73.5</v>
       </c>
       <c r="H50" s="2">
-        <f>E50/F50</f>
+        <f t="shared" si="4"/>
         <v>24.383022774327124</v>
       </c>
       <c r="I50" s="3">
-        <f>E50/(E50+C50)</f>
+        <f t="shared" si="5"/>
         <v>0.29298206333806004</v>
       </c>
       <c r="J50" t="s">
@@ -3241,15 +3241,15 @@
         <v>1384</v>
       </c>
       <c r="G51" s="2">
-        <f>C51/D51</f>
+        <f t="shared" si="3"/>
         <v>78.813084112149539</v>
       </c>
       <c r="H51" s="2">
-        <f>E51/F51</f>
+        <f t="shared" si="4"/>
         <v>15.221098265895954</v>
       </c>
       <c r="I51" s="3">
-        <f>E51/(E51+C51)</f>
+        <f t="shared" si="5"/>
         <v>0.185067074295654</v>
       </c>
       <c r="J51" t="s">
@@ -3279,15 +3279,15 @@
         <v>1297</v>
       </c>
       <c r="G52" s="2">
-        <f>C52/D52</f>
+        <f t="shared" si="3"/>
         <v>67.513182674199626</v>
       </c>
       <c r="H52" s="2">
-        <f>E52/F52</f>
+        <f t="shared" si="4"/>
         <v>16.028527370855819</v>
       </c>
       <c r="I52" s="3">
-        <f>E52/(E52+C52)</f>
+        <f t="shared" si="5"/>
         <v>0.22477510595969208</v>
       </c>
       <c r="J52" t="s">
@@ -3317,15 +3317,15 @@
         <v>1371</v>
       </c>
       <c r="G53" s="2">
-        <f>C53/D53</f>
+        <f t="shared" ref="G53:G83" si="6">C53/D53</f>
         <v>77.431092436974794</v>
       </c>
       <c r="H53" s="2">
-        <f>E53/F53</f>
+        <f t="shared" ref="H53:H83" si="7">E53/F53</f>
         <v>14.843180160466813</v>
       </c>
       <c r="I53" s="3">
-        <f>E53/(E53+C53)</f>
+        <f t="shared" ref="I53:I83" si="8">E53/(E53+C53)</f>
         <v>0.18090014489790476</v>
       </c>
       <c r="J53" t="s">
@@ -3352,15 +3352,15 @@
         <v>1309</v>
       </c>
       <c r="G54" s="2">
-        <f>C54/D54</f>
+        <f t="shared" si="6"/>
         <v>72.430567685589523</v>
       </c>
       <c r="H54" s="2">
-        <f>E54/F54</f>
+        <f t="shared" si="7"/>
         <v>17.064935064935064</v>
       </c>
       <c r="I54" s="3">
-        <f>E54/(E54+C54)</f>
+        <f t="shared" si="8"/>
         <v>0.21219519145823637</v>
       </c>
       <c r="J54" t="s">
@@ -3390,15 +3390,15 @@
         <v>1623</v>
       </c>
       <c r="G55" s="2">
-        <f>C55/D55</f>
+        <f t="shared" si="6"/>
         <v>73.749373433583955</v>
       </c>
       <c r="H55" s="2">
-        <f>E55/F55</f>
+        <f t="shared" si="7"/>
         <v>13.930375847196549</v>
       </c>
       <c r="I55" s="3">
-        <f>E55/(E55+C55)</f>
+        <f t="shared" si="8"/>
         <v>0.20389225066960059</v>
       </c>
       <c r="J55" t="s">
@@ -3428,15 +3428,15 @@
         <v>1354</v>
       </c>
       <c r="G56" s="2">
-        <f>C56/D56</f>
+        <f t="shared" si="6"/>
         <v>75.688424717145338</v>
       </c>
       <c r="H56" s="2">
-        <f>E56/F56</f>
+        <f t="shared" si="7"/>
         <v>18.296898079763665</v>
       </c>
       <c r="I56" s="3">
-        <f>E56/(E56+C56)</f>
+        <f t="shared" si="8"/>
         <v>0.22171111508859853</v>
       </c>
       <c r="J56" t="s">
@@ -3466,15 +3466,15 @@
         <v>1524</v>
       </c>
       <c r="G57" s="2">
-        <f>C57/D57</f>
+        <f t="shared" si="6"/>
         <v>77.69083333333333</v>
       </c>
       <c r="H57" s="2">
-        <f>E57/F57</f>
+        <f t="shared" si="7"/>
         <v>27.961942257217849</v>
       </c>
       <c r="I57" s="3">
-        <f>E57/(E57+C57)</f>
+        <f t="shared" si="8"/>
         <v>0.31370037469726081</v>
       </c>
       <c r="J57" t="s">
@@ -3510,15 +3510,15 @@
         <v>1377</v>
       </c>
       <c r="G58" s="2">
-        <f>C58/D58</f>
+        <f t="shared" si="6"/>
         <v>80.27042965459141</v>
       </c>
       <c r="H58" s="2">
-        <f>E58/F58</f>
+        <f t="shared" si="7"/>
         <v>20.007988380537402</v>
       </c>
       <c r="I58" s="3">
-        <f>E58/(E58+C58)</f>
+        <f t="shared" si="8"/>
         <v>0.22429822847466457</v>
       </c>
       <c r="J58" t="s">
@@ -3554,15 +3554,15 @@
         <v>1417</v>
       </c>
       <c r="G59" s="2">
-        <f>C59/D59</f>
+        <f t="shared" si="6"/>
         <v>76.428082191780817</v>
       </c>
       <c r="H59" s="2">
-        <f>E59/F59</f>
+        <f t="shared" si="7"/>
         <v>26.344389555398731</v>
       </c>
       <c r="I59" s="3">
-        <f>E59/(E59+C59)</f>
+        <f t="shared" si="8"/>
         <v>0.2948703770991643</v>
       </c>
       <c r="J59" t="s">
@@ -3592,15 +3592,15 @@
         <v>1416</v>
       </c>
       <c r="G60" s="2">
-        <f>C60/D60</f>
+        <f t="shared" si="6"/>
         <v>77.849087893864009</v>
       </c>
       <c r="H60" s="2">
-        <f>E60/F60</f>
+        <f t="shared" si="7"/>
         <v>20.645480225988699</v>
       </c>
       <c r="I60" s="3">
-        <f>E60/(E60+C60)</f>
+        <f t="shared" si="8"/>
         <v>0.23744314489928525</v>
       </c>
       <c r="J60" t="s">
@@ -3630,15 +3630,15 @@
         <v>1400</v>
       </c>
       <c r="G61" s="2">
-        <f>C61/D61</f>
+        <f t="shared" si="6"/>
         <v>77.067234042553196</v>
       </c>
       <c r="H61" s="2">
-        <f>E61/F61</f>
+        <f t="shared" si="7"/>
         <v>21.364285714285714</v>
       </c>
       <c r="I61" s="3">
-        <f>E61/(E61+C61)</f>
+        <f t="shared" si="8"/>
         <v>0.24828994554389694</v>
       </c>
       <c r="J61" t="s">
@@ -3668,15 +3668,15 @@
         <v>1441</v>
       </c>
       <c r="G62" s="2">
-        <f>C62/D62</f>
+        <f t="shared" si="6"/>
         <v>74.853043478260872</v>
       </c>
       <c r="H62" s="2">
-        <f>E62/F62</f>
+        <f t="shared" si="7"/>
         <v>26.897293546148507</v>
       </c>
       <c r="I62" s="3">
-        <f>E62/(E62+C62)</f>
+        <f t="shared" si="8"/>
         <v>0.31046940083306634</v>
       </c>
       <c r="J62" t="s">
@@ -3712,15 +3712,15 @@
         <v>1318</v>
       </c>
       <c r="G63" s="2">
-        <f>C63/D63</f>
+        <f t="shared" si="6"/>
         <v>78.685518423307627</v>
       </c>
       <c r="H63" s="2">
-        <f>E63/F63</f>
+        <f t="shared" si="7"/>
         <v>15.517450682852807</v>
       </c>
       <c r="I63" s="3">
-        <f>E63/(E63+C63)</f>
+        <f t="shared" si="8"/>
         <v>0.18215500810488253</v>
       </c>
       <c r="J63" t="s">
@@ -3756,15 +3756,15 @@
         <v>1414</v>
       </c>
       <c r="G64" s="2">
-        <f>C64/D64</f>
+        <f t="shared" si="6"/>
         <v>75.860662701784193</v>
       </c>
       <c r="H64" s="2">
-        <f>E64/F64</f>
+        <f t="shared" si="7"/>
         <v>18.133663366336634</v>
       </c>
       <c r="I64" s="3">
-        <f>E64/(E64+C64)</f>
+        <f t="shared" si="8"/>
         <v>0.22310295921830001</v>
       </c>
       <c r="J64" t="s">
@@ -3794,15 +3794,15 @@
         <v>1381</v>
       </c>
       <c r="G65" s="2">
-        <f>C65/D65</f>
+        <f t="shared" si="6"/>
         <v>78.266291230893003</v>
       </c>
       <c r="H65" s="2">
-        <f>E65/F65</f>
+        <f t="shared" si="7"/>
         <v>10.629978276611151</v>
       </c>
       <c r="I65" s="3">
-        <f>E65/(E65+C65)</f>
+        <f t="shared" si="8"/>
         <v>0.13111240119680256</v>
       </c>
       <c r="J65" t="s">
@@ -3832,15 +3832,15 @@
         <v>1346</v>
       </c>
       <c r="G66" s="2">
-        <f>C66/D66</f>
+        <f t="shared" si="6"/>
         <v>74.460192475940502</v>
       </c>
       <c r="H66" s="2">
-        <f>E66/F66</f>
+        <f t="shared" si="7"/>
         <v>19.398959881129272</v>
       </c>
       <c r="I66" s="3">
-        <f>E66/(E66+C66)</f>
+        <f t="shared" si="8"/>
         <v>0.23477103732275961</v>
       </c>
       <c r="J66" t="s">
@@ -3876,15 +3876,15 @@
         <v>1466</v>
       </c>
       <c r="G67" s="2">
-        <f>C67/D67</f>
+        <f t="shared" si="6"/>
         <v>75.082247557003257</v>
       </c>
       <c r="H67" s="2">
-        <f>E67/F67</f>
+        <f t="shared" si="7"/>
         <v>15.95225102319236</v>
       </c>
       <c r="I67" s="3">
-        <f>E67/(E67+C67)</f>
+        <f t="shared" si="8"/>
         <v>0.20232379073771273</v>
       </c>
       <c r="J67" t="s">
@@ -3920,15 +3920,15 @@
         <v>1306</v>
       </c>
       <c r="G68" s="2">
-        <f>C68/D68</f>
+        <f t="shared" si="6"/>
         <v>66.464318813716403</v>
       </c>
       <c r="H68" s="2">
-        <f>E68/F68</f>
+        <f t="shared" si="7"/>
         <v>14.160796324655436</v>
       </c>
       <c r="I68" s="3">
-        <f>E68/(E68+C68)</f>
+        <f t="shared" si="8"/>
         <v>0.20501280360052768</v>
       </c>
       <c r="J68" t="s">
@@ -3958,15 +3958,15 @@
         <v>1270</v>
       </c>
       <c r="G69" s="2">
-        <f>C69/D69</f>
+        <f t="shared" si="6"/>
         <v>67.77629063097514</v>
       </c>
       <c r="H69" s="2">
-        <f>E69/F69</f>
+        <f t="shared" si="7"/>
         <v>15.545669291338582</v>
       </c>
       <c r="I69" s="3">
-        <f>E69/(E69+C69)</f>
+        <f t="shared" si="8"/>
         <v>0.2178249500755762</v>
       </c>
       <c r="J69" t="s">
@@ -3996,15 +3996,15 @@
         <v>1346</v>
       </c>
       <c r="G70" s="2">
-        <f>C70/D70</f>
+        <f t="shared" si="6"/>
         <v>73.688481675392666</v>
       </c>
       <c r="H70" s="2">
-        <f>E70/F70</f>
+        <f t="shared" si="7"/>
         <v>10.99777117384844</v>
       </c>
       <c r="I70" s="3">
-        <f>E70/(E70+C70)</f>
+        <f t="shared" si="8"/>
         <v>0.14914861460957179</v>
       </c>
       <c r="J70" t="s">
@@ -4034,15 +4034,15 @@
         <v>1457</v>
       </c>
       <c r="G71" s="2">
-        <f>C71/D71</f>
+        <f t="shared" si="6"/>
         <v>75.884552845528461</v>
       </c>
       <c r="H71" s="2">
-        <f>E71/F71</f>
+        <f t="shared" si="7"/>
         <v>11.072752230610844</v>
       </c>
       <c r="I71" s="3">
-        <f>E71/(E71+C71)</f>
+        <f t="shared" si="8"/>
         <v>0.14737236345698862</v>
       </c>
       <c r="J71" t="s">
@@ -4066,15 +4066,15 @@
         <v>1363</v>
       </c>
       <c r="G72" s="2">
-        <f>C72/D72</f>
+        <f t="shared" si="6"/>
         <v>72.778956675508397</v>
       </c>
       <c r="H72" s="2">
-        <f>E72/F72</f>
+        <f t="shared" si="7"/>
         <v>16.430667644900954</v>
       </c>
       <c r="I72" s="3">
-        <f>E72/(E72+C72)</f>
+        <f t="shared" si="8"/>
         <v>0.21388050578752341</v>
       </c>
       <c r="J72" t="s">
@@ -4104,15 +4104,15 @@
         <v>1571</v>
       </c>
       <c r="G73" s="2">
-        <f>C73/D73</f>
+        <f t="shared" si="6"/>
         <v>73.760563380281695</v>
       </c>
       <c r="H73" s="2">
-        <f>E73/F73</f>
+        <f t="shared" si="7"/>
         <v>22.393380012730745</v>
       </c>
       <c r="I73" s="3">
-        <f>E73/(E73+C73)</f>
+        <f t="shared" si="8"/>
         <v>0.28323229395615457</v>
       </c>
       <c r="J73" t="s">
@@ -4142,15 +4142,15 @@
         <v>1327</v>
       </c>
       <c r="G74" s="2">
-        <f>C74/D74</f>
+        <f t="shared" si="6"/>
         <v>78.298723404255313</v>
       </c>
       <c r="H74" s="2">
-        <f>E74/F74</f>
+        <f t="shared" si="7"/>
         <v>17.996232102486811</v>
       </c>
       <c r="I74" s="3">
-        <f>E74/(E74+C74)</f>
+        <f t="shared" si="8"/>
         <v>0.20608032308727844</v>
       </c>
       <c r="J74" t="s">
@@ -4180,15 +4180,15 @@
         <v>1453</v>
       </c>
       <c r="G75" s="2">
-        <f>C75/D75</f>
+        <f t="shared" si="6"/>
         <v>80.348360655737707</v>
       </c>
       <c r="H75" s="2">
-        <f>E75/F75</f>
+        <f t="shared" si="7"/>
         <v>23.709566414315209</v>
       </c>
       <c r="I75" s="3">
-        <f>E75/(E75+C75)</f>
+        <f t="shared" si="8"/>
         <v>0.2600490658614833</v>
       </c>
       <c r="J75" t="s">
@@ -4218,15 +4218,15 @@
         <v>1393</v>
       </c>
       <c r="G76" s="2">
-        <f>C76/D76</f>
+        <f t="shared" si="6"/>
         <v>73.055950266429846</v>
       </c>
       <c r="H76" s="2">
-        <f>E76/F76</f>
+        <f t="shared" si="7"/>
         <v>19.395549174443648</v>
       </c>
       <c r="I76" s="3">
-        <f>E76/(E76+C76)</f>
+        <f t="shared" si="8"/>
         <v>0.24723871924157431</v>
       </c>
       <c r="J76" t="s">
@@ -4262,15 +4262,15 @@
         <v>1376</v>
       </c>
       <c r="G77" s="2">
-        <f>C77/D77</f>
+        <f t="shared" si="6"/>
         <v>76.090757701915066</v>
       </c>
       <c r="H77" s="2">
-        <f>E77/F77</f>
+        <f t="shared" si="7"/>
         <v>12.34811046511628</v>
       </c>
       <c r="I77" s="3">
-        <f>E77/(E77+C77)</f>
+        <f t="shared" si="8"/>
         <v>0.15677825348785709</v>
       </c>
       <c r="J77" t="s">
@@ -4306,15 +4306,15 @@
         <v>1419</v>
       </c>
       <c r="G78" s="2">
-        <f>C78/D78</f>
+        <f t="shared" si="6"/>
         <v>77.356175972927247</v>
       </c>
       <c r="H78" s="2">
-        <f>E78/F78</f>
+        <f t="shared" si="7"/>
         <v>23.687808315715291</v>
       </c>
       <c r="I78" s="3">
-        <f>E78/(E78+C78)</f>
+        <f t="shared" si="8"/>
         <v>0.26880078050028788</v>
       </c>
       <c r="J78" t="s">
@@ -4344,15 +4344,15 @@
         <v>1485</v>
       </c>
       <c r="G79" s="2">
-        <f>C79/D79</f>
+        <f t="shared" si="6"/>
         <v>80.649837133550491</v>
       </c>
       <c r="H79" s="2">
-        <f>E79/F79</f>
+        <f t="shared" si="7"/>
         <v>19.534006734006734</v>
       </c>
       <c r="I79" s="3">
-        <f>E79/(E79+C79)</f>
+        <f t="shared" si="8"/>
         <v>0.22654358589881762</v>
       </c>
       <c r="J79" t="s">
@@ -4382,15 +4382,15 @@
         <v>1503</v>
       </c>
       <c r="G80" s="2">
-        <f>C80/D80</f>
+        <f t="shared" si="6"/>
         <v>73.724455611390283</v>
       </c>
       <c r="H80" s="2">
-        <f>E80/F80</f>
+        <f t="shared" si="7"/>
         <v>21.739188290086492</v>
       </c>
       <c r="I80" s="3">
-        <f>E80/(E80+C80)</f>
+        <f t="shared" si="8"/>
         <v>0.27070198258506556</v>
       </c>
       <c r="J80" t="s">
@@ -4420,15 +4420,15 @@
         <v>1431</v>
       </c>
       <c r="G81" s="2">
-        <f>C81/D81</f>
+        <f t="shared" si="6"/>
         <v>75.196891191709838</v>
       </c>
       <c r="H81" s="2">
-        <f>E81/F81</f>
+        <f t="shared" si="7"/>
         <v>21.964360587002098</v>
       </c>
       <c r="I81" s="3">
-        <f>E81/(E81+C81)</f>
+        <f t="shared" si="8"/>
         <v>0.26522036301040425</v>
       </c>
       <c r="J81" t="s">
@@ -4458,15 +4458,15 @@
         <v>1394</v>
       </c>
       <c r="G82" s="2">
-        <f>C82/D82</f>
+        <f t="shared" si="6"/>
         <v>76.767676767676761</v>
       </c>
       <c r="H82" s="2">
-        <f>E82/F82</f>
+        <f t="shared" si="7"/>
         <v>18.372309899569583</v>
       </c>
       <c r="I82" s="3">
-        <f>E82/(E82+C82)</f>
+        <f t="shared" si="8"/>
         <v>0.21925161157767675</v>
       </c>
       <c r="J82" t="s">
@@ -4496,15 +4496,15 @@
         <v>1447</v>
       </c>
       <c r="G83" s="2">
-        <f>C83/D83</f>
+        <f t="shared" si="6"/>
         <v>77.645747316267546</v>
       </c>
       <c r="H83" s="2">
-        <f>E83/F83</f>
+        <f t="shared" si="7"/>
         <v>19.948168624740845</v>
       </c>
       <c r="I83" s="3">
-        <f>E83/(E83+C83)</f>
+        <f t="shared" si="8"/>
         <v>0.23487721125522809</v>
       </c>
       <c r="J83" t="s">
@@ -7551,15 +7551,15 @@
         <v>1431</v>
       </c>
       <c r="G187" s="2">
-        <f>C187/D187</f>
+        <f t="shared" ref="G187:G202" si="9">C187/D187</f>
         <v>83.231660231660229</v>
       </c>
       <c r="H187" s="2">
-        <f>E187/F187</f>
+        <f t="shared" ref="H187:H202" si="10">E187/F187</f>
         <v>20.073375262054508</v>
       </c>
       <c r="I187" s="3">
-        <f>E187/(E187+C187)</f>
+        <f t="shared" ref="I187:I202" si="11">E187/(E187+C187)</f>
         <v>0.21042414475130028</v>
       </c>
       <c r="J187" t="s">
@@ -7592,15 +7592,15 @@
         <v>1360</v>
       </c>
       <c r="G188" s="2">
-        <f>C188/D188</f>
+        <f t="shared" si="9"/>
         <v>84.011308562197087</v>
       </c>
       <c r="H188" s="2">
-        <f>E188/F188</f>
+        <f t="shared" si="10"/>
         <v>16.646323529411763</v>
       </c>
       <c r="I188" s="3">
-        <f>E188/(E188+C188)</f>
+        <f t="shared" si="11"/>
         <v>0.17875952465553319</v>
       </c>
       <c r="J188" t="s">
@@ -7630,15 +7630,15 @@
         <v>1462</v>
       </c>
       <c r="G189" s="2">
-        <f>C189/D189</f>
+        <f t="shared" si="9"/>
         <v>85.965125094768766</v>
       </c>
       <c r="H189" s="2">
-        <f>E189/F189</f>
+        <f t="shared" si="10"/>
         <v>19.214774281805745</v>
       </c>
       <c r="I189" s="3">
-        <f>E189/(E189+C189)</f>
+        <f t="shared" si="11"/>
         <v>0.19855810008481764</v>
       </c>
       <c r="J189" t="s">
@@ -7668,15 +7668,15 @@
         <v>1452</v>
       </c>
       <c r="G190" s="2">
-        <f>C190/D190</f>
+        <f t="shared" si="9"/>
         <v>84.042721518987335</v>
       </c>
       <c r="H190" s="2">
-        <f>E190/F190</f>
+        <f t="shared" si="10"/>
         <v>19.997245179063359</v>
       </c>
       <c r="I190" s="3">
-        <f>E190/(E190+C190)</f>
+        <f t="shared" si="11"/>
         <v>0.21465852468469535</v>
       </c>
       <c r="J190" t="s">
@@ -7709,15 +7709,15 @@
         <v>1449</v>
       </c>
       <c r="G191" s="2">
-        <f>C191/D191</f>
+        <f t="shared" si="9"/>
         <v>87.95580110497238</v>
       </c>
       <c r="H191" s="2">
-        <f>E191/F191</f>
+        <f t="shared" si="10"/>
         <v>22.722567287784678</v>
       </c>
       <c r="I191" s="3">
-        <f>E191/(E191+C191)</f>
+        <f t="shared" si="11"/>
         <v>0.2280677449520313</v>
       </c>
       <c r="J191" t="s">
@@ -7744,15 +7744,15 @@
         <v>1401</v>
       </c>
       <c r="G192" s="2">
-        <f>C192/D192</f>
+        <f t="shared" si="9"/>
         <v>87.103338632750393</v>
       </c>
       <c r="H192" s="2">
-        <f>E192/F192</f>
+        <f t="shared" si="10"/>
         <v>21.111349036402569</v>
       </c>
       <c r="I192" s="3">
-        <f>E192/(E192+C192)</f>
+        <f t="shared" si="11"/>
         <v>0.21255021451208383</v>
       </c>
       <c r="J192" t="s">
@@ -7779,15 +7779,15 @@
         <v>1446</v>
       </c>
       <c r="G193" s="2">
-        <f>C193/D193</f>
+        <f t="shared" si="9"/>
         <v>78.891376451077946</v>
       </c>
       <c r="H193" s="2">
-        <f>E193/F193</f>
+        <f t="shared" si="10"/>
         <v>24.385200553250346</v>
       </c>
       <c r="I193" s="3">
-        <f>E193/(E193+C193)</f>
+        <f t="shared" si="11"/>
         <v>0.27039814729609524</v>
       </c>
       <c r="J193" t="s">
@@ -7820,15 +7820,15 @@
         <v>1450</v>
       </c>
       <c r="G194" s="2">
-        <f>C194/D194</f>
+        <f t="shared" si="9"/>
         <v>82.915797914995991</v>
       </c>
       <c r="H194" s="2">
-        <f>E194/F194</f>
+        <f t="shared" si="10"/>
         <v>22.177931034482757</v>
       </c>
       <c r="I194" s="3">
-        <f>E194/(E194+C194)</f>
+        <f t="shared" si="11"/>
         <v>0.23723386989686768</v>
       </c>
       <c r="J194" t="s">
@@ -7855,15 +7855,15 @@
         <v>1425</v>
       </c>
       <c r="G195" s="2">
-        <f>C195/D195</f>
+        <f t="shared" si="9"/>
         <v>80.362681744749594</v>
       </c>
       <c r="H195" s="2">
-        <f>E195/F195</f>
+        <f t="shared" si="10"/>
         <v>20.098245614035086</v>
       </c>
       <c r="I195" s="3">
-        <f>E195/(E195+C195)</f>
+        <f t="shared" si="11"/>
         <v>0.22352472898407075</v>
       </c>
       <c r="J195" t="s">
@@ -7890,15 +7890,15 @@
         <v>1038</v>
       </c>
       <c r="G196" s="2">
-        <f>C196/D196</f>
+        <f t="shared" si="9"/>
         <v>55.643757159221074</v>
       </c>
       <c r="H196" s="2">
-        <f>E196/F196</f>
+        <f t="shared" si="10"/>
         <v>9.9412331406551058</v>
       </c>
       <c r="I196" s="3">
-        <f>E196/(E196+C196)</f>
+        <f t="shared" si="11"/>
         <v>0.17520714479760935</v>
       </c>
       <c r="J196" t="s">
@@ -7925,15 +7925,15 @@
         <v>1027</v>
       </c>
       <c r="G197" s="2">
-        <f>C197/D197</f>
+        <f t="shared" si="9"/>
         <v>57.466139954853276</v>
       </c>
       <c r="H197" s="2">
-        <f>E197/F197</f>
+        <f t="shared" si="10"/>
         <v>12.327166504381694</v>
       </c>
       <c r="I197" s="3">
-        <f>E197/(E197+C197)</f>
+        <f t="shared" si="11"/>
         <v>0.19913488006291782</v>
       </c>
       <c r="J197" t="s">
@@ -7960,15 +7960,15 @@
         <v>866</v>
       </c>
       <c r="G198" s="2">
-        <f>C198/D198</f>
+        <f t="shared" si="9"/>
         <v>46.839240506329112</v>
       </c>
       <c r="H198" s="2">
-        <f>E198/F198</f>
+        <f t="shared" si="10"/>
         <v>13.285219399538105</v>
       </c>
       <c r="I198" s="3">
-        <f>E198/(E198+C198)</f>
+        <f t="shared" si="11"/>
         <v>0.23717737280448586</v>
       </c>
       <c r="J198" t="s">
@@ -7995,15 +7995,15 @@
         <v>1133</v>
       </c>
       <c r="G199" s="2">
-        <f>C199/D199</f>
+        <f t="shared" si="9"/>
         <v>63.590214067278289</v>
       </c>
       <c r="H199" s="2">
-        <f>E199/F199</f>
+        <f t="shared" si="10"/>
         <v>12.583406884377759</v>
       </c>
       <c r="I199" s="3">
-        <f>E199/(E199+C199)</f>
+        <f t="shared" si="11"/>
         <v>0.1860280014092042</v>
       </c>
       <c r="J199" t="s">
@@ -8030,15 +8030,15 @@
         <v>1296</v>
       </c>
       <c r="G200" s="2">
-        <f>C200/D200</f>
+        <f t="shared" si="9"/>
         <v>38.403272377285852</v>
       </c>
       <c r="H200" s="2">
-        <f>E200/F200</f>
+        <f t="shared" si="10"/>
         <v>17.897376543209877</v>
       </c>
       <c r="I200" s="3">
-        <f>E200/(E200+C200)</f>
+        <f t="shared" si="11"/>
         <v>0.36761442880689743</v>
       </c>
       <c r="J200" t="s">
@@ -8065,15 +8065,15 @@
         <v>989</v>
       </c>
       <c r="G201" s="2">
-        <f>C201/D201</f>
+        <f t="shared" si="9"/>
         <v>53.277372262773724</v>
       </c>
       <c r="H201" s="2">
-        <f>E201/F201</f>
+        <f t="shared" si="10"/>
         <v>8.5267947421638013</v>
       </c>
       <c r="I201" s="3">
-        <f>E201/(E201+C201)</f>
+        <f t="shared" si="11"/>
         <v>0.16146820610029294</v>
       </c>
       <c r="J201" t="s">
@@ -8100,15 +8100,15 @@
         <v>1383</v>
       </c>
       <c r="G202" s="2">
-        <f>C202/D202</f>
+        <f t="shared" si="9"/>
         <v>26.206576728499158</v>
       </c>
       <c r="H202" s="2">
-        <f>E202/F202</f>
+        <f t="shared" si="10"/>
         <v>18.183658712942879</v>
       </c>
       <c r="I202" s="3">
-        <f>E202/(E202+C202)</f>
+        <f t="shared" si="11"/>
         <v>0.44724252609863235</v>
       </c>
       <c r="J202" t="s">
@@ -8525,6 +8525,9 @@
       </c>
       <c r="F221" s="1">
         <v>1497</v>
+      </c>
+      <c r="J221" t="s">
+        <v>16</v>
       </c>
       <c r="O221" t="s">
         <v>93</v>

</xml_diff>